<commit_message>
Added new tests and experiment results with LDkit
</commit_message>
<xml_diff>
--- a/StatisticalAnalysis/Evaluation Performance DMAOG (final results).xlsx
+++ b/StatisticalAnalysis/Evaluation Performance DMAOG (final results).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
   <si>
     <t>DMAOG</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>LD-flex</t>
+  </si>
+  <si>
+    <t>LDKit</t>
   </si>
   <si>
     <t>All (x100)</t>
@@ -60,6 +63,9 @@
   </si>
   <si>
     <t>LDFlex</t>
+  </si>
+  <si>
+    <t>LDkit</t>
   </si>
 </sst>
 </file>
@@ -329,6 +335,7 @@
     <col customWidth="1" min="6" max="6" width="25.88"/>
     <col customWidth="1" min="7" max="7" width="10.63"/>
     <col customWidth="1" min="8" max="8" width="17.63"/>
+    <col customWidth="1" min="12" max="12" width="17.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -345,35 +352,44 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -405,6 +421,12 @@
       <c r="J3" s="2">
         <v>85405.0</v>
       </c>
+      <c r="K3" s="2">
+        <v>30211.0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>26356.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2"/>
@@ -435,6 +457,12 @@
       <c r="J4" s="2">
         <v>80373.0</v>
       </c>
+      <c r="K4" s="2">
+        <v>32276.0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>25427.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
@@ -465,6 +493,12 @@
       <c r="J5" s="2">
         <v>71526.0</v>
       </c>
+      <c r="K5" s="2">
+        <v>29153.0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>41354.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
@@ -495,6 +529,12 @@
       <c r="J6" s="2">
         <v>81599.0</v>
       </c>
+      <c r="K6" s="2">
+        <v>27197.0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>49674.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
@@ -525,6 +565,12 @@
       <c r="J7" s="2">
         <v>78584.0</v>
       </c>
+      <c r="K7" s="2">
+        <v>27243.0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>46745.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2"/>
@@ -555,6 +601,12 @@
       <c r="J8" s="2">
         <v>78560.0</v>
       </c>
+      <c r="K8" s="2">
+        <v>39635.0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>45535.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2"/>
@@ -585,6 +637,12 @@
       <c r="J9" s="2">
         <v>74029.0</v>
       </c>
+      <c r="K9" s="2">
+        <v>46214.0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>45269.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
@@ -615,6 +673,12 @@
       <c r="J10" s="2">
         <v>75128.0</v>
       </c>
+      <c r="K10" s="2">
+        <v>45354.0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>46616.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
@@ -645,6 +709,12 @@
       <c r="J11" s="2">
         <v>78762.0</v>
       </c>
+      <c r="K11" s="2">
+        <v>48396.0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>48880.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
@@ -675,6 +745,12 @@
       <c r="J12" s="2">
         <v>78018.0</v>
       </c>
+      <c r="K12" s="2">
+        <v>47155.0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>46749.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="2">
@@ -704,6 +780,12 @@
       <c r="J13" s="2">
         <v>78452.0</v>
       </c>
+      <c r="K13" s="2">
+        <v>33749.0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>29423.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="2">
@@ -733,6 +815,12 @@
       <c r="J14" s="2">
         <v>79887.0</v>
       </c>
+      <c r="K14" s="2">
+        <v>31541.0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>30701.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="2">
@@ -762,6 +850,12 @@
       <c r="J15" s="2">
         <v>80761.0</v>
       </c>
+      <c r="K15" s="2">
+        <v>31988.0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>31287.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="2">
@@ -791,6 +885,12 @@
       <c r="J16" s="2">
         <v>78396.0</v>
       </c>
+      <c r="K16" s="2">
+        <v>32092.0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>31662.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="2">
@@ -820,6 +920,12 @@
       <c r="J17" s="2">
         <v>81233.0</v>
       </c>
+      <c r="K17" s="2">
+        <v>28821.0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>30557.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="2">
@@ -849,6 +955,12 @@
       <c r="J18" s="2">
         <v>74037.0</v>
       </c>
+      <c r="K18" s="2">
+        <v>27174.0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>31238.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="2">
@@ -878,6 +990,12 @@
       <c r="J19" s="2">
         <v>82169.0</v>
       </c>
+      <c r="K19" s="2">
+        <v>27146.0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>31726.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="2">
@@ -907,6 +1025,12 @@
       <c r="J20" s="2">
         <v>91023.0</v>
       </c>
+      <c r="K20" s="2">
+        <v>27158.0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>30593.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="2">
@@ -936,6 +1060,12 @@
       <c r="J21" s="2">
         <v>71486.0</v>
       </c>
+      <c r="K21" s="2">
+        <v>27150.0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>29899.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="2">
@@ -965,6 +1095,12 @@
       <c r="J22" s="2">
         <v>76203.0</v>
       </c>
+      <c r="K22" s="2">
+        <v>27022.0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>30103.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="2">
@@ -994,6 +1130,12 @@
       <c r="J23" s="2">
         <v>76784.0</v>
       </c>
+      <c r="K23" s="2">
+        <v>26986.0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>27740.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="2">
@@ -1023,6 +1165,12 @@
       <c r="J24" s="2">
         <v>80285.0</v>
       </c>
+      <c r="K24" s="2">
+        <v>27302.0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>24731.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="2">
@@ -1052,6 +1200,12 @@
       <c r="J25" s="2">
         <v>78436.0</v>
       </c>
+      <c r="K25" s="2">
+        <v>27656.0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>24073.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="2">
@@ -1081,6 +1235,12 @@
       <c r="J26" s="2">
         <v>75911.0</v>
       </c>
+      <c r="K26" s="2">
+        <v>27812.0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>24244.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="2">
@@ -1110,6 +1270,12 @@
       <c r="J27" s="2">
         <v>78907.0</v>
       </c>
+      <c r="K27" s="2">
+        <v>28815.0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>25263.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="2">
@@ -1139,6 +1305,12 @@
       <c r="J28" s="2">
         <v>76147.0</v>
       </c>
+      <c r="K28" s="2">
+        <v>27048.0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>26107.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="2">
@@ -1168,6 +1340,12 @@
       <c r="J29" s="2">
         <v>79160.0</v>
       </c>
+      <c r="K29" s="2">
+        <v>27003.0</v>
+      </c>
+      <c r="L29" s="2">
+        <v>24012.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="2">
@@ -1197,6 +1375,12 @@
       <c r="J30" s="2">
         <v>80220.0</v>
       </c>
+      <c r="K30" s="2">
+        <v>28675.0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>24139.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="2">
@@ -1226,6 +1410,12 @@
       <c r="J31" s="2">
         <v>76167.0</v>
       </c>
+      <c r="K31" s="2">
+        <v>48463.0</v>
+      </c>
+      <c r="L31" s="2">
+        <v>24038.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="2">
@@ -1255,13 +1445,19 @@
       <c r="J32" s="2">
         <v>80004.0</v>
       </c>
+      <c r="K32" s="2">
+        <v>48650.0</v>
+      </c>
+      <c r="L32" s="2">
+        <v>25018.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" ref="B34:J34" si="1">AVERAGE(B3:B32)</f>
+        <f t="shared" ref="B34:L34" si="1">AVERAGE(B3:B32)</f>
         <v>28637.43333</v>
       </c>
       <c r="C34" s="3">
@@ -1296,10 +1492,18 @@
         <f t="shared" si="1"/>
         <v>78588.4</v>
       </c>
+      <c r="K34" s="3">
+        <f t="shared" si="1"/>
+        <v>32836.16667</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" si="1"/>
+        <v>32638.63333</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B35" s="3">
         <f t="shared" ref="B35:C35" si="2">B34/100</f>
@@ -1337,13 +1541,21 @@
         <f t="shared" si="3"/>
         <v>78588.4</v>
       </c>
+      <c r="K35" s="3">
+        <f t="shared" ref="K35:L35" si="4">K34/100</f>
+        <v>328.3616667</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="4"/>
+        <v>326.3863333</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
@@ -1351,11 +1563,11 @@
         <v>0</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" ref="B38:C38" si="4">B35</f>
+        <f t="shared" ref="B38:C38" si="5">B35</f>
         <v>286.3743333</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40.327</v>
       </c>
     </row>
@@ -1377,33 +1589,47 @@
         <v>2</v>
       </c>
       <c r="B40" s="3">
-        <f t="shared" ref="B40:C40" si="5">G35</f>
+        <f t="shared" ref="B40:C40" si="6">G35</f>
         <v>1288.613333</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.9186</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B41" s="3">
-        <f t="shared" ref="B41:C41" si="6">I35</f>
+        <f t="shared" ref="B41:C41" si="7">I35</f>
         <v>330439.2</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78588.4</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" ref="B42:C42" si="8">K35</f>
+        <v>328.3616667</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="8"/>
+        <v>326.3863333</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1439,34 +1665,43 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -1506,6 +1741,14 @@
         <f>Measurements!J3</f>
         <v>85405</v>
       </c>
+      <c r="K3" s="3">
+        <f>Measurements!K3/100</f>
+        <v>302.11</v>
+      </c>
+      <c r="L3" s="3">
+        <f>Measurements!L3/100</f>
+        <v>263.56</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
@@ -1544,6 +1787,14 @@
         <f>Measurements!J4</f>
         <v>80373</v>
       </c>
+      <c r="K4" s="3">
+        <f>Measurements!K4/100</f>
+        <v>322.76</v>
+      </c>
+      <c r="L4" s="3">
+        <f>Measurements!L4/100</f>
+        <v>254.27</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="3">
@@ -1582,6 +1833,14 @@
         <f>Measurements!J5</f>
         <v>71526</v>
       </c>
+      <c r="K5" s="3">
+        <f>Measurements!K5/100</f>
+        <v>291.53</v>
+      </c>
+      <c r="L5" s="3">
+        <f>Measurements!L5/100</f>
+        <v>413.54</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="3">
@@ -1620,6 +1879,14 @@
         <f>Measurements!J6</f>
         <v>81599</v>
       </c>
+      <c r="K6" s="3">
+        <f>Measurements!K6/100</f>
+        <v>271.97</v>
+      </c>
+      <c r="L6" s="3">
+        <f>Measurements!L6/100</f>
+        <v>496.74</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3">
@@ -1658,6 +1925,14 @@
         <f>Measurements!J7</f>
         <v>78584</v>
       </c>
+      <c r="K7" s="3">
+        <f>Measurements!K7/100</f>
+        <v>272.43</v>
+      </c>
+      <c r="L7" s="3">
+        <f>Measurements!L7/100</f>
+        <v>467.45</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="3">
@@ -1696,6 +1971,14 @@
         <f>Measurements!J8</f>
         <v>78560</v>
       </c>
+      <c r="K8" s="3">
+        <f>Measurements!K8/100</f>
+        <v>396.35</v>
+      </c>
+      <c r="L8" s="3">
+        <f>Measurements!L8/100</f>
+        <v>455.35</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="3">
@@ -1734,6 +2017,14 @@
         <f>Measurements!J9</f>
         <v>74029</v>
       </c>
+      <c r="K9" s="3">
+        <f>Measurements!K9/100</f>
+        <v>462.14</v>
+      </c>
+      <c r="L9" s="3">
+        <f>Measurements!L9/100</f>
+        <v>452.69</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="3">
@@ -1772,6 +2063,14 @@
         <f>Measurements!J10</f>
         <v>75128</v>
       </c>
+      <c r="K10" s="3">
+        <f>Measurements!K10/100</f>
+        <v>453.54</v>
+      </c>
+      <c r="L10" s="3">
+        <f>Measurements!L10/100</f>
+        <v>466.16</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="3">
@@ -1810,6 +2109,14 @@
         <f>Measurements!J11</f>
         <v>78762</v>
       </c>
+      <c r="K11" s="3">
+        <f>Measurements!K11/100</f>
+        <v>483.96</v>
+      </c>
+      <c r="L11" s="3">
+        <f>Measurements!L11/100</f>
+        <v>488.8</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="3">
@@ -1848,6 +2155,14 @@
         <f>Measurements!J12</f>
         <v>78018</v>
       </c>
+      <c r="K12" s="3">
+        <f>Measurements!K12/100</f>
+        <v>471.55</v>
+      </c>
+      <c r="L12" s="3">
+        <f>Measurements!L12/100</f>
+        <v>467.49</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="3">
@@ -1886,6 +2201,14 @@
         <f>Measurements!J13</f>
         <v>78452</v>
       </c>
+      <c r="K13" s="3">
+        <f>Measurements!K13/100</f>
+        <v>337.49</v>
+      </c>
+      <c r="L13" s="3">
+        <f>Measurements!L13/100</f>
+        <v>294.23</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="3">
@@ -1924,6 +2247,14 @@
         <f>Measurements!J14</f>
         <v>79887</v>
       </c>
+      <c r="K14" s="3">
+        <f>Measurements!K14/100</f>
+        <v>315.41</v>
+      </c>
+      <c r="L14" s="3">
+        <f>Measurements!L14/100</f>
+        <v>307.01</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="3">
@@ -1962,6 +2293,14 @@
         <f>Measurements!J15</f>
         <v>80761</v>
       </c>
+      <c r="K15" s="3">
+        <f>Measurements!K15/100</f>
+        <v>319.88</v>
+      </c>
+      <c r="L15" s="3">
+        <f>Measurements!L15/100</f>
+        <v>312.87</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="3">
@@ -2000,6 +2339,14 @@
         <f>Measurements!J16</f>
         <v>78396</v>
       </c>
+      <c r="K16" s="3">
+        <f>Measurements!K16/100</f>
+        <v>320.92</v>
+      </c>
+      <c r="L16" s="3">
+        <f>Measurements!L16/100</f>
+        <v>316.62</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="3">
@@ -2038,6 +2385,14 @@
         <f>Measurements!J17</f>
         <v>81233</v>
       </c>
+      <c r="K17" s="3">
+        <f>Measurements!K17/100</f>
+        <v>288.21</v>
+      </c>
+      <c r="L17" s="3">
+        <f>Measurements!L17/100</f>
+        <v>305.57</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="3">
@@ -2076,6 +2431,14 @@
         <f>Measurements!J18</f>
         <v>74037</v>
       </c>
+      <c r="K18" s="3">
+        <f>Measurements!K18/100</f>
+        <v>271.74</v>
+      </c>
+      <c r="L18" s="3">
+        <f>Measurements!L18/100</f>
+        <v>312.38</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="3">
@@ -2114,6 +2477,14 @@
         <f>Measurements!J19</f>
         <v>82169</v>
       </c>
+      <c r="K19" s="3">
+        <f>Measurements!K19/100</f>
+        <v>271.46</v>
+      </c>
+      <c r="L19" s="3">
+        <f>Measurements!L19/100</f>
+        <v>317.26</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="3">
@@ -2152,6 +2523,14 @@
         <f>Measurements!J20</f>
         <v>91023</v>
       </c>
+      <c r="K20" s="3">
+        <f>Measurements!K20/100</f>
+        <v>271.58</v>
+      </c>
+      <c r="L20" s="3">
+        <f>Measurements!L20/100</f>
+        <v>305.93</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="3">
@@ -2190,6 +2569,14 @@
         <f>Measurements!J21</f>
         <v>71486</v>
       </c>
+      <c r="K21" s="3">
+        <f>Measurements!K21/100</f>
+        <v>271.5</v>
+      </c>
+      <c r="L21" s="3">
+        <f>Measurements!L21/100</f>
+        <v>298.99</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="3">
@@ -2228,6 +2615,14 @@
         <f>Measurements!J22</f>
         <v>76203</v>
       </c>
+      <c r="K22" s="3">
+        <f>Measurements!K22/100</f>
+        <v>270.22</v>
+      </c>
+      <c r="L22" s="3">
+        <f>Measurements!L22/100</f>
+        <v>301.03</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="3">
@@ -2266,6 +2661,14 @@
         <f>Measurements!J23</f>
         <v>76784</v>
       </c>
+      <c r="K23" s="3">
+        <f>Measurements!K23/100</f>
+        <v>269.86</v>
+      </c>
+      <c r="L23" s="3">
+        <f>Measurements!L23/100</f>
+        <v>277.4</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="3">
@@ -2304,6 +2707,14 @@
         <f>Measurements!J24</f>
         <v>80285</v>
       </c>
+      <c r="K24" s="3">
+        <f>Measurements!K24/100</f>
+        <v>273.02</v>
+      </c>
+      <c r="L24" s="3">
+        <f>Measurements!L24/100</f>
+        <v>247.31</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="3">
@@ -2342,6 +2753,14 @@
         <f>Measurements!J25</f>
         <v>78436</v>
       </c>
+      <c r="K25" s="3">
+        <f>Measurements!K25/100</f>
+        <v>276.56</v>
+      </c>
+      <c r="L25" s="3">
+        <f>Measurements!L25/100</f>
+        <v>240.73</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="3">
@@ -2380,6 +2799,14 @@
         <f>Measurements!J26</f>
         <v>75911</v>
       </c>
+      <c r="K26" s="3">
+        <f>Measurements!K26/100</f>
+        <v>278.12</v>
+      </c>
+      <c r="L26" s="3">
+        <f>Measurements!L26/100</f>
+        <v>242.44</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="3">
@@ -2418,6 +2845,14 @@
         <f>Measurements!J27</f>
         <v>78907</v>
       </c>
+      <c r="K27" s="3">
+        <f>Measurements!K27/100</f>
+        <v>288.15</v>
+      </c>
+      <c r="L27" s="3">
+        <f>Measurements!L27/100</f>
+        <v>252.63</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="3">
@@ -2456,6 +2891,14 @@
         <f>Measurements!J28</f>
         <v>76147</v>
       </c>
+      <c r="K28" s="3">
+        <f>Measurements!K28/100</f>
+        <v>270.48</v>
+      </c>
+      <c r="L28" s="3">
+        <f>Measurements!L28/100</f>
+        <v>261.07</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="3">
@@ -2494,6 +2937,14 @@
         <f>Measurements!J29</f>
         <v>79160</v>
       </c>
+      <c r="K29" s="3">
+        <f>Measurements!K29/100</f>
+        <v>270.03</v>
+      </c>
+      <c r="L29" s="3">
+        <f>Measurements!L29/100</f>
+        <v>240.12</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="3">
@@ -2532,6 +2983,14 @@
         <f>Measurements!J30</f>
         <v>80220</v>
       </c>
+      <c r="K30" s="3">
+        <f>Measurements!K30/100</f>
+        <v>286.75</v>
+      </c>
+      <c r="L30" s="3">
+        <f>Measurements!L30/100</f>
+        <v>241.39</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="3">
@@ -2570,6 +3029,14 @@
         <f>Measurements!J31</f>
         <v>76167</v>
       </c>
+      <c r="K31" s="3">
+        <f>Measurements!K31/100</f>
+        <v>484.63</v>
+      </c>
+      <c r="L31" s="3">
+        <f>Measurements!L31/100</f>
+        <v>240.38</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="3">
@@ -2608,13 +3075,21 @@
         <f>Measurements!J32</f>
         <v>80004</v>
       </c>
+      <c r="K32" s="3">
+        <f>Measurements!K32/100</f>
+        <v>486.5</v>
+      </c>
+      <c r="L32" s="3">
+        <f>Measurements!L32/100</f>
+        <v>250.18</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" ref="B34:J34" si="1">AVERAGE(B3:B32)</f>
+        <f t="shared" ref="B34:L34" si="1">AVERAGE(B3:B32)</f>
         <v>286.3743333</v>
       </c>
       <c r="C34" s="3">
@@ -2649,13 +3124,21 @@
         <f t="shared" si="1"/>
         <v>78588.4</v>
       </c>
+      <c r="K34" s="3">
+        <f t="shared" si="1"/>
+        <v>328.3616667</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" si="1"/>
+        <v>326.3863333</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
@@ -2699,7 +3182,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B41" s="3">
         <f t="shared" ref="B41:C41" si="4">I34</f>
@@ -2708,6 +3191,19 @@
       <c r="C41" s="3">
         <f t="shared" si="4"/>
         <v>78588.4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="3">
+        <f t="shared" ref="B42:C42" si="5">K34</f>
+        <v>328.3616667</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="5"/>
+        <v>326.3863333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel/tabular version of results
</commit_message>
<xml_diff>
--- a/StatisticalAnalysis/Evaluation Performance DMAOG (final results).xlsx
+++ b/StatisticalAnalysis/Evaluation Performance DMAOG (final results).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
   <si>
     <t>DMAOG</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>LDKit</t>
+  </si>
+  <si>
+    <t>LDO</t>
   </si>
   <si>
     <t>All (x100)</t>
@@ -54,6 +57,9 @@
   </si>
   <si>
     <t>Search by field</t>
+  </si>
+  <si>
+    <t>Search by field (x10)</t>
   </si>
   <si>
     <t>Mean</t>
@@ -336,6 +342,8 @@
     <col customWidth="1" min="7" max="7" width="10.63"/>
     <col customWidth="1" min="8" max="8" width="17.63"/>
     <col customWidth="1" min="12" max="12" width="17.63"/>
+    <col customWidth="1" min="13" max="13" width="14.13"/>
+    <col customWidth="1" min="14" max="14" width="17.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -355,41 +363,50 @@
       <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>6</v>
+      <c r="N2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -427,6 +444,12 @@
       <c r="L3" s="2">
         <v>26356.0</v>
       </c>
+      <c r="M3" s="2">
+        <v>85176.0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>96733.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2"/>
@@ -463,6 +486,12 @@
       <c r="L4" s="2">
         <v>25427.0</v>
       </c>
+      <c r="M4" s="2">
+        <v>136841.0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>87338.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
@@ -499,6 +528,12 @@
       <c r="L5" s="2">
         <v>41354.0</v>
       </c>
+      <c r="M5" s="2">
+        <v>140538.0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>83164.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
@@ -535,6 +570,12 @@
       <c r="L6" s="2">
         <v>49674.0</v>
       </c>
+      <c r="M6" s="2">
+        <v>153926.0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>86164.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
@@ -571,6 +612,12 @@
       <c r="L7" s="2">
         <v>46745.0</v>
       </c>
+      <c r="M7" s="2">
+        <v>134612.0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>139007.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2"/>
@@ -607,6 +654,12 @@
       <c r="L8" s="2">
         <v>45535.0</v>
       </c>
+      <c r="M8" s="2">
+        <v>134404.0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>142816.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2"/>
@@ -643,6 +696,12 @@
       <c r="L9" s="2">
         <v>45269.0</v>
       </c>
+      <c r="M9" s="2">
+        <v>146178.0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>136489.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
@@ -679,6 +738,12 @@
       <c r="L10" s="2">
         <v>46616.0</v>
       </c>
+      <c r="M10" s="2">
+        <v>92668.0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>73988.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
@@ -715,6 +780,12 @@
       <c r="L11" s="2">
         <v>48880.0</v>
       </c>
+      <c r="M11" s="2">
+        <v>87608.0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>87560.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
@@ -751,6 +822,12 @@
       <c r="L12" s="2">
         <v>46749.0</v>
       </c>
+      <c r="M12" s="2">
+        <v>84667.0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>85673.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="2">
@@ -786,6 +863,12 @@
       <c r="L13" s="2">
         <v>29423.0</v>
       </c>
+      <c r="M13" s="2">
+        <v>90568.0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>79656.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="2">
@@ -821,6 +904,12 @@
       <c r="L14" s="2">
         <v>30701.0</v>
       </c>
+      <c r="M14" s="2">
+        <v>81995.0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>87141.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="2">
@@ -856,6 +945,12 @@
       <c r="L15" s="2">
         <v>31287.0</v>
       </c>
+      <c r="M15" s="2">
+        <v>88636.0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>103710.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="2">
@@ -891,6 +986,12 @@
       <c r="L16" s="2">
         <v>31662.0</v>
       </c>
+      <c r="M16" s="2">
+        <v>93807.0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>96920.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="2">
@@ -926,6 +1027,12 @@
       <c r="L17" s="2">
         <v>30557.0</v>
       </c>
+      <c r="M17" s="2">
+        <v>90939.0</v>
+      </c>
+      <c r="N17" s="2">
+        <v>93466.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="2">
@@ -961,6 +1068,12 @@
       <c r="L18" s="2">
         <v>31238.0</v>
       </c>
+      <c r="M18" s="2">
+        <v>93874.0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>114054.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="2">
@@ -996,6 +1109,12 @@
       <c r="L19" s="2">
         <v>31726.0</v>
       </c>
+      <c r="M19" s="2">
+        <v>79731.0</v>
+      </c>
+      <c r="N19" s="2">
+        <v>144549.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="2">
@@ -1031,6 +1150,12 @@
       <c r="L20" s="2">
         <v>30593.0</v>
       </c>
+      <c r="M20" s="2">
+        <v>88113.0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>141329.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="2">
@@ -1066,6 +1191,12 @@
       <c r="L21" s="2">
         <v>29899.0</v>
       </c>
+      <c r="M21" s="2">
+        <v>96339.0</v>
+      </c>
+      <c r="N21" s="2">
+        <v>122245.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="2">
@@ -1101,6 +1232,12 @@
       <c r="L22" s="2">
         <v>30103.0</v>
       </c>
+      <c r="M22" s="2">
+        <v>153680.0</v>
+      </c>
+      <c r="N22" s="2">
+        <v>74876.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="2">
@@ -1136,6 +1273,12 @@
       <c r="L23" s="2">
         <v>27740.0</v>
       </c>
+      <c r="M23" s="2">
+        <v>155191.0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>79253.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="2">
@@ -1171,6 +1314,12 @@
       <c r="L24" s="2">
         <v>24731.0</v>
       </c>
+      <c r="M24" s="2">
+        <v>148634.0</v>
+      </c>
+      <c r="N24" s="2">
+        <v>95503.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="2">
@@ -1206,6 +1355,12 @@
       <c r="L25" s="2">
         <v>24073.0</v>
       </c>
+      <c r="M25" s="2">
+        <v>94082.0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>140581.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="2">
@@ -1241,6 +1396,12 @@
       <c r="L26" s="2">
         <v>24244.0</v>
       </c>
+      <c r="M26" s="2">
+        <v>85646.0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>119424.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="2">
@@ -1276,6 +1437,12 @@
       <c r="L27" s="2">
         <v>25263.0</v>
       </c>
+      <c r="M27" s="2">
+        <v>86120.0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>133458.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="2">
@@ -1311,6 +1478,12 @@
       <c r="L28" s="2">
         <v>26107.0</v>
       </c>
+      <c r="M28" s="2">
+        <v>85762.0</v>
+      </c>
+      <c r="N28" s="2">
+        <v>86205.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="2">
@@ -1346,6 +1519,12 @@
       <c r="L29" s="2">
         <v>24012.0</v>
       </c>
+      <c r="M29" s="2">
+        <v>114049.0</v>
+      </c>
+      <c r="N29" s="2">
+        <v>140420.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="2">
@@ -1381,6 +1560,12 @@
       <c r="L30" s="2">
         <v>24139.0</v>
       </c>
+      <c r="M30" s="2">
+        <v>87131.0</v>
+      </c>
+      <c r="N30" s="2">
+        <v>139410.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="2">
@@ -1416,6 +1601,12 @@
       <c r="L31" s="2">
         <v>24038.0</v>
       </c>
+      <c r="M31" s="2">
+        <v>87708.0</v>
+      </c>
+      <c r="N31" s="2">
+        <v>140638.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="2">
@@ -1451,13 +1642,19 @@
       <c r="L32" s="2">
         <v>25018.0</v>
       </c>
+      <c r="M32" s="2">
+        <v>108679.0</v>
+      </c>
+      <c r="N32" s="2">
+        <v>104916.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" ref="B34:L34" si="1">AVERAGE(B3:B32)</f>
+        <f t="shared" ref="B34:N34" si="1">AVERAGE(B3:B32)</f>
         <v>28637.43333</v>
       </c>
       <c r="C34" s="3">
@@ -1500,10 +1697,18 @@
         <f t="shared" si="1"/>
         <v>32638.63333</v>
       </c>
+      <c r="M34" s="3">
+        <f t="shared" si="1"/>
+        <v>106910.0667</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" si="1"/>
+        <v>108556.2</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B35" s="3">
         <f t="shared" ref="B35:C35" si="2">B34/100</f>
@@ -1549,13 +1754,21 @@
         <f t="shared" si="4"/>
         <v>326.3863333</v>
       </c>
+      <c r="M35" s="3">
+        <f t="shared" ref="M35:N35" si="5">M34/10</f>
+        <v>10691.00667</v>
+      </c>
+      <c r="N35" s="3">
+        <f t="shared" si="5"/>
+        <v>10855.62</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38">
@@ -1563,11 +1776,11 @@
         <v>0</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" ref="B38:C38" si="5">B35</f>
+        <f t="shared" ref="B38:C38" si="6">B35</f>
         <v>286.3743333</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40.327</v>
       </c>
     </row>
@@ -1589,47 +1802,61 @@
         <v>2</v>
       </c>
       <c r="B40" s="3">
-        <f t="shared" ref="B40:C40" si="6">G35</f>
+        <f t="shared" ref="B40:C40" si="7">G35</f>
         <v>1288.613333</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.9186</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B41" s="3">
-        <f t="shared" ref="B41:C41" si="7">I35</f>
+        <f t="shared" ref="B41:C41" si="8">I35</f>
         <v>330439.2</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>78588.4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B42" s="3">
-        <f t="shared" ref="B42:C42" si="8">K35</f>
+        <f t="shared" ref="B42:C42" si="9">K35</f>
         <v>328.3616667</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>326.3863333</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" ref="B43:C43" si="10">M35</f>
+        <v>10691.00667</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="10"/>
+        <v>10855.62</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1650,6 +1877,8 @@
     <col customWidth="1" min="6" max="6" width="28.63"/>
     <col customWidth="1" min="8" max="8" width="17.5"/>
     <col customWidth="1" min="9" max="9" width="13.75"/>
+    <col customWidth="1" min="12" max="12" width="18.0"/>
+    <col customWidth="1" min="14" max="14" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1665,43 +1894,52 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>6</v>
+      <c r="N2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -1749,6 +1987,14 @@
         <f>Measurements!L3/100</f>
         <v>263.56</v>
       </c>
+      <c r="M3" s="3">
+        <f>Measurements!M3/10</f>
+        <v>8517.6</v>
+      </c>
+      <c r="N3" s="3">
+        <f>Measurements!N3/10</f>
+        <v>9673.3</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
@@ -1795,6 +2041,14 @@
         <f>Measurements!L4/100</f>
         <v>254.27</v>
       </c>
+      <c r="M4" s="3">
+        <f>Measurements!M4/10</f>
+        <v>13684.1</v>
+      </c>
+      <c r="N4" s="3">
+        <f>Measurements!N4/10</f>
+        <v>8733.8</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="3">
@@ -1841,6 +2095,14 @@
         <f>Measurements!L5/100</f>
         <v>413.54</v>
       </c>
+      <c r="M5" s="3">
+        <f>Measurements!M5/10</f>
+        <v>14053.8</v>
+      </c>
+      <c r="N5" s="3">
+        <f>Measurements!N5/10</f>
+        <v>8316.4</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="3">
@@ -1887,6 +2149,14 @@
         <f>Measurements!L6/100</f>
         <v>496.74</v>
       </c>
+      <c r="M6" s="3">
+        <f>Measurements!M6/10</f>
+        <v>15392.6</v>
+      </c>
+      <c r="N6" s="3">
+        <f>Measurements!N6/10</f>
+        <v>8616.4</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="3">
@@ -1933,6 +2203,14 @@
         <f>Measurements!L7/100</f>
         <v>467.45</v>
       </c>
+      <c r="M7" s="3">
+        <f>Measurements!M7/10</f>
+        <v>13461.2</v>
+      </c>
+      <c r="N7" s="3">
+        <f>Measurements!N7/10</f>
+        <v>13900.7</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="3">
@@ -1979,6 +2257,14 @@
         <f>Measurements!L8/100</f>
         <v>455.35</v>
       </c>
+      <c r="M8" s="3">
+        <f>Measurements!M8/10</f>
+        <v>13440.4</v>
+      </c>
+      <c r="N8" s="3">
+        <f>Measurements!N8/10</f>
+        <v>14281.6</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="3">
@@ -2025,6 +2311,14 @@
         <f>Measurements!L9/100</f>
         <v>452.69</v>
       </c>
+      <c r="M9" s="3">
+        <f>Measurements!M9/10</f>
+        <v>14617.8</v>
+      </c>
+      <c r="N9" s="3">
+        <f>Measurements!N9/10</f>
+        <v>13648.9</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="3">
@@ -2071,6 +2365,14 @@
         <f>Measurements!L10/100</f>
         <v>466.16</v>
       </c>
+      <c r="M10" s="3">
+        <f>Measurements!M10/10</f>
+        <v>9266.8</v>
+      </c>
+      <c r="N10" s="3">
+        <f>Measurements!N10/10</f>
+        <v>7398.8</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" s="3">
@@ -2117,6 +2419,14 @@
         <f>Measurements!L11/100</f>
         <v>488.8</v>
       </c>
+      <c r="M11" s="3">
+        <f>Measurements!M11/10</f>
+        <v>8760.8</v>
+      </c>
+      <c r="N11" s="3">
+        <f>Measurements!N11/10</f>
+        <v>8756</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="3">
@@ -2163,6 +2473,14 @@
         <f>Measurements!L12/100</f>
         <v>467.49</v>
       </c>
+      <c r="M12" s="3">
+        <f>Measurements!M12/10</f>
+        <v>8466.7</v>
+      </c>
+      <c r="N12" s="3">
+        <f>Measurements!N12/10</f>
+        <v>8567.3</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" s="3">
@@ -2209,6 +2527,14 @@
         <f>Measurements!L13/100</f>
         <v>294.23</v>
       </c>
+      <c r="M13" s="3">
+        <f>Measurements!M13/10</f>
+        <v>9056.8</v>
+      </c>
+      <c r="N13" s="3">
+        <f>Measurements!N13/10</f>
+        <v>7965.6</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" s="3">
@@ -2255,6 +2581,14 @@
         <f>Measurements!L14/100</f>
         <v>307.01</v>
       </c>
+      <c r="M14" s="3">
+        <f>Measurements!M14/10</f>
+        <v>8199.5</v>
+      </c>
+      <c r="N14" s="3">
+        <f>Measurements!N14/10</f>
+        <v>8714.1</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="3">
@@ -2301,6 +2635,14 @@
         <f>Measurements!L15/100</f>
         <v>312.87</v>
       </c>
+      <c r="M15" s="3">
+        <f>Measurements!M15/10</f>
+        <v>8863.6</v>
+      </c>
+      <c r="N15" s="3">
+        <f>Measurements!N15/10</f>
+        <v>10371</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="3">
@@ -2347,6 +2689,14 @@
         <f>Measurements!L16/100</f>
         <v>316.62</v>
       </c>
+      <c r="M16" s="3">
+        <f>Measurements!M16/10</f>
+        <v>9380.7</v>
+      </c>
+      <c r="N16" s="3">
+        <f>Measurements!N16/10</f>
+        <v>9692</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="3">
@@ -2393,6 +2743,14 @@
         <f>Measurements!L17/100</f>
         <v>305.57</v>
       </c>
+      <c r="M17" s="3">
+        <f>Measurements!M17/10</f>
+        <v>9093.9</v>
+      </c>
+      <c r="N17" s="3">
+        <f>Measurements!N17/10</f>
+        <v>9346.6</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="3">
@@ -2439,6 +2797,14 @@
         <f>Measurements!L18/100</f>
         <v>312.38</v>
       </c>
+      <c r="M18" s="3">
+        <f>Measurements!M18/10</f>
+        <v>9387.4</v>
+      </c>
+      <c r="N18" s="3">
+        <f>Measurements!N18/10</f>
+        <v>11405.4</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" s="3">
@@ -2485,6 +2851,14 @@
         <f>Measurements!L19/100</f>
         <v>317.26</v>
       </c>
+      <c r="M19" s="3">
+        <f>Measurements!M19/10</f>
+        <v>7973.1</v>
+      </c>
+      <c r="N19" s="3">
+        <f>Measurements!N19/10</f>
+        <v>14454.9</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="3">
@@ -2531,6 +2905,14 @@
         <f>Measurements!L20/100</f>
         <v>305.93</v>
       </c>
+      <c r="M20" s="3">
+        <f>Measurements!M20/10</f>
+        <v>8811.3</v>
+      </c>
+      <c r="N20" s="3">
+        <f>Measurements!N20/10</f>
+        <v>14132.9</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="3">
@@ -2577,6 +2959,14 @@
         <f>Measurements!L21/100</f>
         <v>298.99</v>
       </c>
+      <c r="M21" s="3">
+        <f>Measurements!M21/10</f>
+        <v>9633.9</v>
+      </c>
+      <c r="N21" s="3">
+        <f>Measurements!N21/10</f>
+        <v>12224.5</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" s="3">
@@ -2623,6 +3013,14 @@
         <f>Measurements!L22/100</f>
         <v>301.03</v>
       </c>
+      <c r="M22" s="3">
+        <f>Measurements!M22/10</f>
+        <v>15368</v>
+      </c>
+      <c r="N22" s="3">
+        <f>Measurements!N22/10</f>
+        <v>7487.6</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" s="3">
@@ -2669,6 +3067,14 @@
         <f>Measurements!L23/100</f>
         <v>277.4</v>
       </c>
+      <c r="M23" s="3">
+        <f>Measurements!M23/10</f>
+        <v>15519.1</v>
+      </c>
+      <c r="N23" s="3">
+        <f>Measurements!N23/10</f>
+        <v>7925.3</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" s="3">
@@ -2715,6 +3121,14 @@
         <f>Measurements!L24/100</f>
         <v>247.31</v>
       </c>
+      <c r="M24" s="3">
+        <f>Measurements!M24/10</f>
+        <v>14863.4</v>
+      </c>
+      <c r="N24" s="3">
+        <f>Measurements!N24/10</f>
+        <v>9550.3</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="3">
@@ -2761,6 +3175,14 @@
         <f>Measurements!L25/100</f>
         <v>240.73</v>
       </c>
+      <c r="M25" s="3">
+        <f>Measurements!M25/10</f>
+        <v>9408.2</v>
+      </c>
+      <c r="N25" s="3">
+        <f>Measurements!N25/10</f>
+        <v>14058.1</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" s="3">
@@ -2807,6 +3229,14 @@
         <f>Measurements!L26/100</f>
         <v>242.44</v>
       </c>
+      <c r="M26" s="3">
+        <f>Measurements!M26/10</f>
+        <v>8564.6</v>
+      </c>
+      <c r="N26" s="3">
+        <f>Measurements!N26/10</f>
+        <v>11942.4</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="3">
@@ -2853,6 +3283,14 @@
         <f>Measurements!L27/100</f>
         <v>252.63</v>
       </c>
+      <c r="M27" s="3">
+        <f>Measurements!M27/10</f>
+        <v>8612</v>
+      </c>
+      <c r="N27" s="3">
+        <f>Measurements!N27/10</f>
+        <v>13345.8</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" s="3">
@@ -2899,6 +3337,14 @@
         <f>Measurements!L28/100</f>
         <v>261.07</v>
       </c>
+      <c r="M28" s="3">
+        <f>Measurements!M28/10</f>
+        <v>8576.2</v>
+      </c>
+      <c r="N28" s="3">
+        <f>Measurements!N28/10</f>
+        <v>8620.5</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" s="3">
@@ -2945,6 +3391,14 @@
         <f>Measurements!L29/100</f>
         <v>240.12</v>
       </c>
+      <c r="M29" s="3">
+        <f>Measurements!M29/10</f>
+        <v>11404.9</v>
+      </c>
+      <c r="N29" s="3">
+        <f>Measurements!N29/10</f>
+        <v>14042</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" s="3">
@@ -2991,6 +3445,14 @@
         <f>Measurements!L30/100</f>
         <v>241.39</v>
       </c>
+      <c r="M30" s="3">
+        <f>Measurements!M30/10</f>
+        <v>8713.1</v>
+      </c>
+      <c r="N30" s="3">
+        <f>Measurements!N30/10</f>
+        <v>13941</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="3">
@@ -3037,6 +3499,14 @@
         <f>Measurements!L31/100</f>
         <v>240.38</v>
       </c>
+      <c r="M31" s="3">
+        <f>Measurements!M31/10</f>
+        <v>8770.8</v>
+      </c>
+      <c r="N31" s="3">
+        <f>Measurements!N31/10</f>
+        <v>14063.8</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" s="3">
@@ -3083,13 +3553,21 @@
         <f>Measurements!L32/100</f>
         <v>250.18</v>
       </c>
+      <c r="M32" s="3">
+        <f>Measurements!M32/10</f>
+        <v>10867.9</v>
+      </c>
+      <c r="N32" s="3">
+        <f>Measurements!N32/10</f>
+        <v>10491.6</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" ref="B34:L34" si="1">AVERAGE(B3:B32)</f>
+        <f t="shared" ref="B34:N34" si="1">AVERAGE(B3:B32)</f>
         <v>286.3743333</v>
       </c>
       <c r="C34" s="3">
@@ -3132,13 +3610,21 @@
         <f t="shared" si="1"/>
         <v>326.3863333</v>
       </c>
+      <c r="M34" s="3">
+        <f t="shared" si="1"/>
+        <v>10691.00667</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" si="1"/>
+        <v>10855.62</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38">
@@ -3182,7 +3668,7 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B41" s="3">
         <f t="shared" ref="B41:C41" si="4">I34</f>
@@ -3195,7 +3681,7 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B42" s="3">
         <f t="shared" ref="B42:C42" si="5">K34</f>
@@ -3206,12 +3692,27 @@
         <v>326.3863333</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="3">
+        <f t="shared" ref="B43:C43" si="6">M34</f>
+        <v>10691.00667</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="6"/>
+        <v>10855.62</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed to LDkit 2.0.0 and consequently updated the statistical analysis
</commit_message>
<xml_diff>
--- a/StatisticalAnalysis/Evaluation Performance DMAOG (final results).xlsx
+++ b/StatisticalAnalysis/Evaluation Performance DMAOG (final results).xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Herminio\Desktop\ExamplesDMAOGPaper\StatisticalAnalysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17715" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Measurements" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Normalised measurements" sheetId="2" r:id="rId5"/>
+    <sheet name="Measurements" sheetId="1" r:id="rId1"/>
+    <sheet name="Normalised measurements" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -77,15 +85,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -96,44 +105,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -323,51 +339,63 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="18.13"/>
-    <col customWidth="1" min="5" max="5" width="49.25"/>
-    <col customWidth="1" min="6" max="6" width="25.88"/>
-    <col customWidth="1" min="7" max="7" width="10.63"/>
-    <col customWidth="1" min="8" max="8" width="17.63"/>
-    <col customWidth="1" min="12" max="12" width="17.63"/>
-    <col customWidth="1" min="13" max="13" width="14.13"/>
-    <col customWidth="1" min="14" max="14" width="17.13"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="5"/>
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -400,7 +428,7 @@
         <v>6</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>11</v>
@@ -409,1322 +437,1322 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2">
-        <v>19153.0</v>
+        <v>19153</v>
       </c>
       <c r="C3" s="2">
-        <v>4589.0</v>
+        <v>4589</v>
       </c>
       <c r="D3" s="2">
-        <v>190184.0</v>
+        <v>190184</v>
       </c>
       <c r="E3" s="2">
-        <v>4937.0</v>
+        <v>4937</v>
       </c>
       <c r="F3" s="2">
-        <v>197449.0</v>
+        <v>197449</v>
       </c>
       <c r="G3" s="2">
-        <v>13641.0</v>
+        <v>13641</v>
       </c>
       <c r="H3" s="2">
-        <v>7454.0</v>
+        <v>7454</v>
       </c>
       <c r="I3" s="2">
-        <v>454724.0</v>
+        <v>454724</v>
       </c>
       <c r="J3" s="2">
-        <v>85405.0</v>
+        <v>85405</v>
       </c>
       <c r="K3" s="2">
-        <v>30211.0</v>
+        <v>15703</v>
       </c>
       <c r="L3" s="2">
-        <v>26356.0</v>
+        <v>6200</v>
       </c>
       <c r="M3" s="2">
-        <v>85176.0</v>
+        <v>85176</v>
       </c>
       <c r="N3" s="2">
-        <v>96733.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>96733</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2">
-        <v>20205.0</v>
+        <v>20205</v>
       </c>
       <c r="C4" s="2">
-        <v>3591.0</v>
+        <v>3591</v>
       </c>
       <c r="D4" s="2">
-        <v>185939.0</v>
+        <v>185939</v>
       </c>
       <c r="E4" s="2">
-        <v>4799.0</v>
+        <v>4799</v>
       </c>
       <c r="F4" s="2">
-        <v>126015.0</v>
+        <v>126015</v>
       </c>
       <c r="G4" s="2">
-        <v>13413.0</v>
+        <v>13413</v>
       </c>
       <c r="H4" s="2">
-        <v>6069.0</v>
+        <v>6069</v>
       </c>
       <c r="I4" s="2">
-        <v>447694.0</v>
+        <v>447694</v>
       </c>
       <c r="J4" s="2">
-        <v>80373.0</v>
+        <v>80373</v>
       </c>
       <c r="K4" s="2">
-        <v>32276.0</v>
+        <v>14873</v>
       </c>
       <c r="L4" s="2">
-        <v>25427.0</v>
+        <v>5741</v>
       </c>
       <c r="M4" s="2">
-        <v>136841.0</v>
+        <v>136841</v>
       </c>
       <c r="N4" s="2">
-        <v>87338.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>87338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2">
-        <v>30021.0</v>
+        <v>30021</v>
       </c>
       <c r="C5" s="2">
-        <v>4053.0</v>
+        <v>4053</v>
       </c>
       <c r="D5" s="2">
-        <v>190021.0</v>
+        <v>190021</v>
       </c>
       <c r="E5" s="2">
-        <v>4703.0</v>
+        <v>4703</v>
       </c>
       <c r="F5" s="2">
-        <v>102906.0</v>
+        <v>102906</v>
       </c>
       <c r="G5" s="2">
-        <v>13108.0</v>
+        <v>13108</v>
       </c>
       <c r="H5" s="2">
-        <v>5437.0</v>
+        <v>5437</v>
       </c>
       <c r="I5" s="2">
-        <v>367957.0</v>
+        <v>367957</v>
       </c>
       <c r="J5" s="2">
-        <v>71526.0</v>
+        <v>71526</v>
       </c>
       <c r="K5" s="2">
-        <v>29153.0</v>
+        <v>16505</v>
       </c>
       <c r="L5" s="2">
-        <v>41354.0</v>
+        <v>6383</v>
       </c>
       <c r="M5" s="2">
-        <v>140538.0</v>
+        <v>140538</v>
       </c>
       <c r="N5" s="2">
-        <v>83164.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>83164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2">
-        <v>29936.0</v>
+        <v>29936</v>
       </c>
       <c r="C6" s="2">
-        <v>3667.0</v>
+        <v>3667</v>
       </c>
       <c r="D6" s="2">
-        <v>157883.0</v>
+        <v>157883</v>
       </c>
       <c r="E6" s="2">
-        <v>4948.0</v>
+        <v>4948</v>
       </c>
       <c r="F6" s="2">
-        <v>102907.0</v>
+        <v>102907</v>
       </c>
       <c r="G6" s="2">
-        <v>12882.0</v>
+        <v>12882</v>
       </c>
       <c r="H6" s="2">
-        <v>5423.0</v>
+        <v>5423</v>
       </c>
       <c r="I6" s="2">
-        <v>475638.0</v>
+        <v>475638</v>
       </c>
       <c r="J6" s="2">
-        <v>81599.0</v>
+        <v>81599</v>
       </c>
       <c r="K6" s="2">
-        <v>27197.0</v>
+        <v>14648</v>
       </c>
       <c r="L6" s="2">
-        <v>49674.0</v>
+        <v>6758</v>
       </c>
       <c r="M6" s="2">
-        <v>153926.0</v>
+        <v>153926</v>
       </c>
       <c r="N6" s="2">
-        <v>86164.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>86164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2">
-        <v>31983.0</v>
+        <v>31983</v>
       </c>
       <c r="C7" s="2">
-        <v>3786.0</v>
+        <v>3786</v>
       </c>
       <c r="D7" s="2">
-        <v>107816.0</v>
+        <v>107816</v>
       </c>
       <c r="E7" s="2">
-        <v>4907.0</v>
+        <v>4907</v>
       </c>
       <c r="F7" s="2">
-        <v>102228.0</v>
+        <v>102228</v>
       </c>
       <c r="G7" s="2">
-        <v>12893.0</v>
+        <v>12893</v>
       </c>
       <c r="H7" s="2">
-        <v>5689.0</v>
+        <v>5689</v>
       </c>
       <c r="I7" s="2">
-        <v>491882.0</v>
+        <v>491882</v>
       </c>
       <c r="J7" s="2">
-        <v>78584.0</v>
+        <v>78584</v>
       </c>
       <c r="K7" s="2">
-        <v>27243.0</v>
+        <v>15209</v>
       </c>
       <c r="L7" s="2">
-        <v>46745.0</v>
+        <v>6028</v>
       </c>
       <c r="M7" s="2">
-        <v>134612.0</v>
+        <v>134612</v>
       </c>
       <c r="N7" s="2">
-        <v>139007.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>139007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2">
-        <v>28462.0</v>
+        <v>28462</v>
       </c>
       <c r="C8" s="2">
-        <v>3477.0</v>
+        <v>3477</v>
       </c>
       <c r="D8" s="2">
-        <v>100433.0</v>
+        <v>100433</v>
       </c>
       <c r="E8" s="2">
-        <v>5128.0</v>
+        <v>5128</v>
       </c>
       <c r="F8" s="2">
-        <v>97661.0</v>
+        <v>97661</v>
       </c>
       <c r="G8" s="2">
-        <v>12890.0</v>
+        <v>12890</v>
       </c>
       <c r="H8" s="2">
-        <v>7347.0</v>
+        <v>7347</v>
       </c>
       <c r="I8" s="2">
-        <v>456532.0</v>
+        <v>456532</v>
       </c>
       <c r="J8" s="2">
-        <v>78560.0</v>
+        <v>78560</v>
       </c>
       <c r="K8" s="2">
-        <v>39635.0</v>
+        <v>14891</v>
       </c>
       <c r="L8" s="2">
-        <v>45535.0</v>
+        <v>5029</v>
       </c>
       <c r="M8" s="2">
-        <v>134404.0</v>
+        <v>134404</v>
       </c>
       <c r="N8" s="2">
-        <v>142816.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>142816</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2">
-        <v>30200.0</v>
+        <v>30200</v>
       </c>
       <c r="C9" s="2">
-        <v>4153.0</v>
+        <v>4153</v>
       </c>
       <c r="D9" s="2">
-        <v>94618.0</v>
+        <v>94618</v>
       </c>
       <c r="E9" s="2">
-        <v>5278.0</v>
+        <v>5278</v>
       </c>
       <c r="F9" s="2">
-        <v>95807.0</v>
+        <v>95807</v>
       </c>
       <c r="G9" s="2">
-        <v>12721.0</v>
+        <v>12721</v>
       </c>
       <c r="H9" s="2">
-        <v>8228.0</v>
+        <v>8228</v>
       </c>
       <c r="I9" s="2">
-        <v>270423.0</v>
+        <v>270423</v>
       </c>
       <c r="J9" s="2">
-        <v>74029.0</v>
+        <v>74029</v>
       </c>
       <c r="K9" s="2">
-        <v>46214.0</v>
+        <v>16938</v>
       </c>
       <c r="L9" s="2">
-        <v>45269.0</v>
+        <v>5233</v>
       </c>
       <c r="M9" s="2">
-        <v>146178.0</v>
+        <v>146178</v>
       </c>
       <c r="N9" s="2">
-        <v>136489.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>136489</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2">
-        <v>31869.0</v>
+        <v>31869</v>
       </c>
       <c r="C10" s="2">
-        <v>3835.0</v>
+        <v>3835</v>
       </c>
       <c r="D10" s="2">
-        <v>94551.0</v>
+        <v>94551</v>
       </c>
       <c r="E10" s="2">
-        <v>5023.0</v>
+        <v>5023</v>
       </c>
       <c r="F10" s="2">
-        <v>102293.0</v>
+        <v>102293</v>
       </c>
       <c r="G10" s="2">
-        <v>12958.0</v>
+        <v>12958</v>
       </c>
       <c r="H10" s="2">
-        <v>8001.0</v>
+        <v>8001</v>
       </c>
       <c r="I10" s="2">
-        <v>257988.0</v>
+        <v>257988</v>
       </c>
       <c r="J10" s="2">
-        <v>75128.0</v>
+        <v>75128</v>
       </c>
       <c r="K10" s="2">
-        <v>45354.0</v>
+        <v>20885</v>
       </c>
       <c r="L10" s="2">
-        <v>46616.0</v>
+        <v>5632</v>
       </c>
       <c r="M10" s="2">
-        <v>92668.0</v>
+        <v>92668</v>
       </c>
       <c r="N10" s="2">
-        <v>73988.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>73988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2">
-        <v>31113.0</v>
+        <v>31113</v>
       </c>
       <c r="C11" s="2">
-        <v>3827.0</v>
+        <v>3827</v>
       </c>
       <c r="D11" s="2">
-        <v>113557.0</v>
+        <v>113557</v>
       </c>
       <c r="E11" s="2">
-        <v>4857.0</v>
+        <v>4857</v>
       </c>
       <c r="F11" s="2">
-        <v>104951.0</v>
+        <v>104951</v>
       </c>
       <c r="G11" s="2">
-        <v>12949.0</v>
+        <v>12949</v>
       </c>
       <c r="H11" s="2">
-        <v>8026.0</v>
+        <v>8026</v>
       </c>
       <c r="I11" s="2">
-        <v>254766.0</v>
+        <v>254766</v>
       </c>
       <c r="J11" s="2">
-        <v>78762.0</v>
+        <v>78762</v>
       </c>
       <c r="K11" s="2">
-        <v>48396.0</v>
+        <v>19795</v>
       </c>
       <c r="L11" s="2">
-        <v>48880.0</v>
+        <v>6707</v>
       </c>
       <c r="M11" s="2">
-        <v>87608.0</v>
+        <v>87608</v>
       </c>
       <c r="N11" s="2">
-        <v>87560.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>87560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2">
-        <v>30973.0</v>
+        <v>30973</v>
       </c>
       <c r="C12" s="2">
-        <v>3726.0</v>
+        <v>3726</v>
       </c>
       <c r="D12" s="2">
-        <v>96818.0</v>
+        <v>96818</v>
       </c>
       <c r="E12" s="2">
-        <v>4739.0</v>
+        <v>4739</v>
       </c>
       <c r="F12" s="2">
-        <v>103913.0</v>
+        <v>103913</v>
       </c>
       <c r="G12" s="2">
-        <v>12827.0</v>
+        <v>12827</v>
       </c>
       <c r="H12" s="2">
-        <v>7944.0</v>
+        <v>7944</v>
       </c>
       <c r="I12" s="2">
-        <v>259544.0</v>
+        <v>259544</v>
       </c>
       <c r="J12" s="2">
-        <v>78018.0</v>
+        <v>78018</v>
       </c>
       <c r="K12" s="2">
-        <v>47155.0</v>
+        <v>17525</v>
       </c>
       <c r="L12" s="2">
-        <v>46749.0</v>
+        <v>6791</v>
       </c>
       <c r="M12" s="2">
-        <v>84667.0</v>
+        <v>84667</v>
       </c>
       <c r="N12" s="2">
-        <v>85673.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>85673</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
-        <v>30453.0</v>
+        <v>30453</v>
       </c>
       <c r="C13" s="2">
-        <v>4151.0</v>
+        <v>4151</v>
       </c>
       <c r="D13" s="2">
-        <v>97566.0</v>
+        <v>97566</v>
       </c>
       <c r="E13" s="2">
-        <v>4958.0</v>
+        <v>4958</v>
       </c>
       <c r="F13" s="2">
-        <v>100573.0</v>
+        <v>100573</v>
       </c>
       <c r="G13" s="2">
-        <v>13149.0</v>
+        <v>13149</v>
       </c>
       <c r="H13" s="2">
-        <v>7904.0</v>
+        <v>7904</v>
       </c>
       <c r="I13" s="2">
-        <v>256665.0</v>
+        <v>256665</v>
       </c>
       <c r="J13" s="2">
-        <v>78452.0</v>
+        <v>78452</v>
       </c>
       <c r="K13" s="2">
-        <v>33749.0</v>
+        <v>16201</v>
       </c>
       <c r="L13" s="2">
-        <v>29423.0</v>
+        <v>6839</v>
       </c>
       <c r="M13" s="2">
-        <v>90568.0</v>
+        <v>90568</v>
       </c>
       <c r="N13" s="2">
-        <v>79656.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>79656</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
-        <v>30736.0</v>
+        <v>30736</v>
       </c>
       <c r="C14" s="2">
-        <v>3498.0</v>
+        <v>3498</v>
       </c>
       <c r="D14" s="2">
-        <v>97262.0</v>
+        <v>97262</v>
       </c>
       <c r="E14" s="2">
-        <v>4970.0</v>
+        <v>4970</v>
       </c>
       <c r="F14" s="2">
-        <v>103365.0</v>
+        <v>103365</v>
       </c>
       <c r="G14" s="2">
-        <v>12596.0</v>
+        <v>12596</v>
       </c>
       <c r="H14" s="2">
-        <v>8118.0</v>
+        <v>8118</v>
       </c>
       <c r="I14" s="2">
-        <v>258985.0</v>
+        <v>258985</v>
       </c>
       <c r="J14" s="2">
-        <v>79887.0</v>
+        <v>79887</v>
       </c>
       <c r="K14" s="2">
-        <v>31541.0</v>
+        <v>14705</v>
       </c>
       <c r="L14" s="2">
-        <v>30701.0</v>
+        <v>6603</v>
       </c>
       <c r="M14" s="2">
-        <v>81995.0</v>
+        <v>81995</v>
       </c>
       <c r="N14" s="2">
-        <v>87141.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>87141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
-        <v>30884.0</v>
+        <v>30884</v>
       </c>
       <c r="C15" s="2">
-        <v>3946.0</v>
+        <v>3946</v>
       </c>
       <c r="D15" s="2">
-        <v>94509.0</v>
+        <v>94509</v>
       </c>
       <c r="E15" s="2">
-        <v>4783.0</v>
+        <v>4783</v>
       </c>
       <c r="F15" s="2">
-        <v>100642.0</v>
+        <v>100642</v>
       </c>
       <c r="G15" s="2">
-        <v>12410.0</v>
+        <v>12410</v>
       </c>
       <c r="H15" s="2">
-        <v>7883.0</v>
+        <v>7883</v>
       </c>
       <c r="I15" s="2">
-        <v>297808.0</v>
+        <v>297808</v>
       </c>
       <c r="J15" s="2">
-        <v>80761.0</v>
+        <v>80761</v>
       </c>
       <c r="K15" s="2">
-        <v>31988.0</v>
+        <v>14603</v>
       </c>
       <c r="L15" s="2">
-        <v>31287.0</v>
+        <v>6543</v>
       </c>
       <c r="M15" s="2">
-        <v>88636.0</v>
+        <v>88636</v>
       </c>
       <c r="N15" s="2">
-        <v>103710.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>103710</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
-        <v>28539.0</v>
+        <v>28539</v>
       </c>
       <c r="C16" s="2">
-        <v>3776.0</v>
+        <v>3776</v>
       </c>
       <c r="D16" s="2">
-        <v>94660.0</v>
+        <v>94660</v>
       </c>
       <c r="E16" s="2">
-        <v>4643.0</v>
+        <v>4643</v>
       </c>
       <c r="F16" s="2">
-        <v>96485.0</v>
+        <v>96485</v>
       </c>
       <c r="G16" s="2">
-        <v>12644.0</v>
+        <v>12644</v>
       </c>
       <c r="H16" s="2">
-        <v>8175.0</v>
+        <v>8175</v>
       </c>
       <c r="I16" s="2">
-        <v>344496.0</v>
+        <v>344496</v>
       </c>
       <c r="J16" s="2">
-        <v>78396.0</v>
+        <v>78396</v>
       </c>
       <c r="K16" s="2">
-        <v>32092.0</v>
+        <v>14719</v>
       </c>
       <c r="L16" s="2">
-        <v>31662.0</v>
+        <v>6527</v>
       </c>
       <c r="M16" s="2">
-        <v>93807.0</v>
+        <v>93807</v>
       </c>
       <c r="N16" s="2">
-        <v>96920.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>96920</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
-        <v>24456.0</v>
+        <v>24456</v>
       </c>
       <c r="C17" s="2">
-        <v>4000.0</v>
+        <v>4000</v>
       </c>
       <c r="D17" s="2">
-        <v>94683.0</v>
+        <v>94683</v>
       </c>
       <c r="E17" s="2">
-        <v>5202.0</v>
+        <v>5202</v>
       </c>
       <c r="F17" s="2">
-        <v>99228.0</v>
+        <v>99228</v>
       </c>
       <c r="G17" s="2">
-        <v>12590.0</v>
+        <v>12590</v>
       </c>
       <c r="H17" s="2">
-        <v>8339.0</v>
+        <v>8339</v>
       </c>
       <c r="I17" s="2">
-        <v>468067.0</v>
+        <v>468067</v>
       </c>
       <c r="J17" s="2">
-        <v>81233.0</v>
+        <v>81233</v>
       </c>
       <c r="K17" s="2">
-        <v>28821.0</v>
+        <v>14712</v>
       </c>
       <c r="L17" s="2">
-        <v>30557.0</v>
+        <v>7027</v>
       </c>
       <c r="M17" s="2">
-        <v>90939.0</v>
+        <v>90939</v>
       </c>
       <c r="N17" s="2">
-        <v>93466.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>93466</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
-        <v>28176.0</v>
+        <v>28176</v>
       </c>
       <c r="C18" s="2">
-        <v>3969.0</v>
+        <v>3969</v>
       </c>
       <c r="D18" s="2">
-        <v>104504.0</v>
+        <v>104504</v>
       </c>
       <c r="E18" s="2">
-        <v>5179.0</v>
+        <v>5179</v>
       </c>
       <c r="F18" s="2">
-        <v>103522.0</v>
+        <v>103522</v>
       </c>
       <c r="G18" s="2">
-        <v>13291.0</v>
+        <v>13291</v>
       </c>
       <c r="H18" s="2">
-        <v>8275.0</v>
+        <v>8275</v>
       </c>
       <c r="I18" s="2">
-        <v>464795.0</v>
+        <v>464795</v>
       </c>
       <c r="J18" s="2">
-        <v>74037.0</v>
+        <v>74037</v>
       </c>
       <c r="K18" s="2">
-        <v>27174.0</v>
+        <v>14945</v>
       </c>
       <c r="L18" s="2">
-        <v>31238.0</v>
+        <v>6739</v>
       </c>
       <c r="M18" s="2">
-        <v>93874.0</v>
+        <v>93874</v>
       </c>
       <c r="N18" s="2">
-        <v>114054.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>114054</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
-        <v>29428.0</v>
+        <v>29428</v>
       </c>
       <c r="C19" s="2">
-        <v>3753.0</v>
+        <v>3753</v>
       </c>
       <c r="D19" s="2">
-        <v>107973.0</v>
+        <v>107973</v>
       </c>
       <c r="E19" s="2">
-        <v>4948.0</v>
+        <v>4948</v>
       </c>
       <c r="F19" s="2">
-        <v>103031.0</v>
+        <v>103031</v>
       </c>
       <c r="G19" s="2">
-        <v>12740.0</v>
+        <v>12740</v>
       </c>
       <c r="H19" s="2">
-        <v>8298.0</v>
+        <v>8298</v>
       </c>
       <c r="I19" s="2">
-        <v>453070.0</v>
+        <v>453070</v>
       </c>
       <c r="J19" s="2">
-        <v>82169.0</v>
+        <v>82169</v>
       </c>
       <c r="K19" s="2">
-        <v>27146.0</v>
+        <v>15761</v>
       </c>
       <c r="L19" s="2">
-        <v>31726.0</v>
+        <v>6951</v>
       </c>
       <c r="M19" s="2">
-        <v>79731.0</v>
+        <v>79731</v>
       </c>
       <c r="N19" s="2">
-        <v>144549.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>144549</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
-        <v>31680.0</v>
+        <v>31680</v>
       </c>
       <c r="C20" s="2">
-        <v>4454.0</v>
+        <v>4454</v>
       </c>
       <c r="D20" s="2">
-        <v>99653.0</v>
+        <v>99653</v>
       </c>
       <c r="E20" s="2">
-        <v>4992.0</v>
+        <v>4992</v>
       </c>
       <c r="F20" s="2">
-        <v>101546.0</v>
+        <v>101546</v>
       </c>
       <c r="G20" s="2">
-        <v>12955.0</v>
+        <v>12955</v>
       </c>
       <c r="H20" s="2">
-        <v>8956.0</v>
+        <v>8956</v>
       </c>
       <c r="I20" s="2">
-        <v>473191.0</v>
+        <v>473191</v>
       </c>
       <c r="J20" s="2">
-        <v>91023.0</v>
+        <v>91023</v>
       </c>
       <c r="K20" s="2">
-        <v>27158.0</v>
+        <v>15864</v>
       </c>
       <c r="L20" s="2">
-        <v>30593.0</v>
+        <v>6721</v>
       </c>
       <c r="M20" s="2">
-        <v>88113.0</v>
+        <v>88113</v>
       </c>
       <c r="N20" s="2">
-        <v>141329.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>141329</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
-        <v>30175.0</v>
+        <v>30175</v>
       </c>
       <c r="C21" s="2">
-        <v>4361.0</v>
+        <v>4361</v>
       </c>
       <c r="D21" s="2">
-        <v>94860.0</v>
+        <v>94860</v>
       </c>
       <c r="E21" s="2">
-        <v>4920.0</v>
+        <v>4920</v>
       </c>
       <c r="F21" s="2">
-        <v>179579.0</v>
+        <v>179579</v>
       </c>
       <c r="G21" s="2">
-        <v>12813.0</v>
+        <v>12813</v>
       </c>
       <c r="H21" s="2">
-        <v>8289.0</v>
+        <v>8289</v>
       </c>
       <c r="I21" s="2">
-        <v>451403.0</v>
+        <v>451403</v>
       </c>
       <c r="J21" s="2">
-        <v>71486.0</v>
+        <v>71486</v>
       </c>
       <c r="K21" s="2">
-        <v>27150.0</v>
+        <v>15921</v>
       </c>
       <c r="L21" s="2">
-        <v>29899.0</v>
+        <v>6996</v>
       </c>
       <c r="M21" s="2">
-        <v>96339.0</v>
+        <v>96339</v>
       </c>
       <c r="N21" s="2">
-        <v>122245.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>122245</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
-        <v>29399.0</v>
+        <v>29399</v>
       </c>
       <c r="C22" s="2">
-        <v>4492.0</v>
+        <v>4492</v>
       </c>
       <c r="D22" s="2">
-        <v>110331.0</v>
+        <v>110331</v>
       </c>
       <c r="E22" s="2">
-        <v>4968.0</v>
+        <v>4968</v>
       </c>
       <c r="F22" s="2">
-        <v>190375.0</v>
+        <v>190375</v>
       </c>
       <c r="G22" s="2">
-        <v>13016.0</v>
+        <v>13016</v>
       </c>
       <c r="H22" s="2">
-        <v>8329.0</v>
+        <v>8329</v>
       </c>
       <c r="I22" s="2">
-        <v>297463.0</v>
+        <v>297463</v>
       </c>
       <c r="J22" s="2">
-        <v>76203.0</v>
+        <v>76203</v>
       </c>
       <c r="K22" s="2">
-        <v>27022.0</v>
+        <v>15613</v>
       </c>
       <c r="L22" s="2">
-        <v>30103.0</v>
+        <v>6906</v>
       </c>
       <c r="M22" s="2">
-        <v>153680.0</v>
+        <v>153680</v>
       </c>
       <c r="N22" s="2">
-        <v>74876.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>74876</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
-        <v>29247.0</v>
+        <v>29247</v>
       </c>
       <c r="C23" s="2">
-        <v>4273.0</v>
+        <v>4273</v>
       </c>
       <c r="D23" s="2">
-        <v>126051.0</v>
+        <v>126051</v>
       </c>
       <c r="E23" s="2">
-        <v>4790.0</v>
+        <v>4790</v>
       </c>
       <c r="F23" s="2">
-        <v>192440.0</v>
+        <v>192440</v>
       </c>
       <c r="G23" s="2">
-        <v>14094.0</v>
+        <v>14094</v>
       </c>
       <c r="H23" s="2">
-        <v>8110.0</v>
+        <v>8110</v>
       </c>
       <c r="I23" s="2">
-        <v>256584.0</v>
+        <v>256584</v>
       </c>
       <c r="J23" s="2">
-        <v>76784.0</v>
+        <v>76784</v>
       </c>
       <c r="K23" s="2">
-        <v>26986.0</v>
+        <v>15928</v>
       </c>
       <c r="L23" s="2">
-        <v>27740.0</v>
+        <v>6890</v>
       </c>
       <c r="M23" s="2">
-        <v>155191.0</v>
+        <v>155191</v>
       </c>
       <c r="N23" s="2">
-        <v>79253.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>79253</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
-        <v>28845.0</v>
+        <v>28845</v>
       </c>
       <c r="C24" s="2">
-        <v>4585.0</v>
+        <v>4585</v>
       </c>
       <c r="D24" s="2">
-        <v>100523.0</v>
+        <v>100523</v>
       </c>
       <c r="E24" s="2">
-        <v>4895.0</v>
+        <v>4895</v>
       </c>
       <c r="F24" s="2">
-        <v>196168.0</v>
+        <v>196168</v>
       </c>
       <c r="G24" s="2">
-        <v>12949.0</v>
+        <v>12949</v>
       </c>
       <c r="H24" s="2">
-        <v>8517.0</v>
+        <v>8517</v>
       </c>
       <c r="I24" s="2">
-        <v>250073.0</v>
+        <v>250073</v>
       </c>
       <c r="J24" s="2">
-        <v>80285.0</v>
+        <v>80285</v>
       </c>
       <c r="K24" s="2">
-        <v>27302.0</v>
+        <v>15741</v>
       </c>
       <c r="L24" s="2">
-        <v>24731.0</v>
+        <v>6569</v>
       </c>
       <c r="M24" s="2">
-        <v>148634.0</v>
+        <v>148634</v>
       </c>
       <c r="N24" s="2">
-        <v>95503.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>95503</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
-        <v>30048.0</v>
+        <v>30048</v>
       </c>
       <c r="C25" s="2">
-        <v>4324.0</v>
+        <v>4324</v>
       </c>
       <c r="D25" s="2">
-        <v>108056.0</v>
+        <v>108056</v>
       </c>
       <c r="E25" s="2">
-        <v>4878.0</v>
+        <v>4878</v>
       </c>
       <c r="F25" s="2">
-        <v>189681.0</v>
+        <v>189681</v>
       </c>
       <c r="G25" s="2">
-        <v>12766.0</v>
+        <v>12766</v>
       </c>
       <c r="H25" s="2">
-        <v>8424.0</v>
+        <v>8424</v>
       </c>
       <c r="I25" s="2">
-        <v>238677.0</v>
+        <v>238677</v>
       </c>
       <c r="J25" s="2">
-        <v>78436.0</v>
+        <v>78436</v>
       </c>
       <c r="K25" s="2">
-        <v>27656.0</v>
+        <v>15753</v>
       </c>
       <c r="L25" s="2">
-        <v>24073.0</v>
+        <v>6504</v>
       </c>
       <c r="M25" s="2">
-        <v>94082.0</v>
+        <v>94082</v>
       </c>
       <c r="N25" s="2">
-        <v>140581.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>140581</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
-        <v>29354.0</v>
+        <v>29354</v>
       </c>
       <c r="C26" s="2">
-        <v>4314.0</v>
+        <v>4314</v>
       </c>
       <c r="D26" s="2">
-        <v>102003.0</v>
+        <v>102003</v>
       </c>
       <c r="E26" s="2">
-        <v>5114.0</v>
+        <v>5114</v>
       </c>
       <c r="F26" s="2">
-        <v>146343.0</v>
+        <v>146343</v>
       </c>
       <c r="G26" s="2">
-        <v>12616.0</v>
+        <v>12616</v>
       </c>
       <c r="H26" s="2">
-        <v>8510.0</v>
+        <v>8510</v>
       </c>
       <c r="I26" s="2">
-        <v>238486.0</v>
+        <v>238486</v>
       </c>
       <c r="J26" s="2">
-        <v>75911.0</v>
+        <v>75911</v>
       </c>
       <c r="K26" s="2">
-        <v>27812.0</v>
+        <v>15855</v>
       </c>
       <c r="L26" s="2">
-        <v>24244.0</v>
+        <v>6895</v>
       </c>
       <c r="M26" s="2">
-        <v>85646.0</v>
+        <v>85646</v>
       </c>
       <c r="N26" s="2">
-        <v>119424.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>119424</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
-        <v>29769.0</v>
+        <v>29769</v>
       </c>
       <c r="C27" s="2">
-        <v>4241.0</v>
+        <v>4241</v>
       </c>
       <c r="D27" s="2">
-        <v>187256.0</v>
+        <v>187256</v>
       </c>
       <c r="E27" s="2">
-        <v>4932.0</v>
+        <v>4932</v>
       </c>
       <c r="F27" s="2">
-        <v>100137.0</v>
+        <v>100137</v>
       </c>
       <c r="G27" s="2">
-        <v>12808.0</v>
+        <v>12808</v>
       </c>
       <c r="H27" s="2">
-        <v>8482.0</v>
+        <v>8482</v>
       </c>
       <c r="I27" s="2">
-        <v>237357.0</v>
+        <v>237357</v>
       </c>
       <c r="J27" s="2">
-        <v>78907.0</v>
+        <v>78907</v>
       </c>
       <c r="K27" s="2">
-        <v>28815.0</v>
+        <v>16114</v>
       </c>
       <c r="L27" s="2">
-        <v>25263.0</v>
+        <v>6809</v>
       </c>
       <c r="M27" s="2">
-        <v>86120.0</v>
+        <v>86120</v>
       </c>
       <c r="N27" s="2">
-        <v>133458.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>133458</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
-        <v>27925.0</v>
+        <v>27925</v>
       </c>
       <c r="C28" s="2">
-        <v>4200.0</v>
+        <v>4200</v>
       </c>
       <c r="D28" s="2">
-        <v>186261.0</v>
+        <v>186261</v>
       </c>
       <c r="E28" s="2">
-        <v>4778.0</v>
+        <v>4778</v>
       </c>
       <c r="F28" s="2">
-        <v>98614.0</v>
+        <v>98614</v>
       </c>
       <c r="G28" s="2">
-        <v>12810.0</v>
+        <v>12810</v>
       </c>
       <c r="H28" s="2">
-        <v>8847.0</v>
+        <v>8847</v>
       </c>
       <c r="I28" s="2">
-        <v>238073.0</v>
+        <v>238073</v>
       </c>
       <c r="J28" s="2">
-        <v>76147.0</v>
+        <v>76147</v>
       </c>
       <c r="K28" s="2">
-        <v>27048.0</v>
+        <v>16246</v>
       </c>
       <c r="L28" s="2">
-        <v>26107.0</v>
+        <v>6646</v>
       </c>
       <c r="M28" s="2">
-        <v>85762.0</v>
+        <v>85762</v>
       </c>
       <c r="N28" s="2">
-        <v>86205.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>86205</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
-        <v>21287.0</v>
+        <v>21287</v>
       </c>
       <c r="C29" s="2">
-        <v>3579.0</v>
+        <v>3579</v>
       </c>
       <c r="D29" s="2">
-        <v>191510.0</v>
+        <v>191510</v>
       </c>
       <c r="E29" s="2">
-        <v>4828.0</v>
+        <v>4828</v>
       </c>
       <c r="F29" s="2">
-        <v>103178.0</v>
+        <v>103178</v>
       </c>
       <c r="G29" s="2">
-        <v>12607.0</v>
+        <v>12607</v>
       </c>
       <c r="H29" s="2">
-        <v>8158.0</v>
+        <v>8158</v>
       </c>
       <c r="I29" s="2">
-        <v>237190.0</v>
+        <v>237190</v>
       </c>
       <c r="J29" s="2">
-        <v>79160.0</v>
+        <v>79160</v>
       </c>
       <c r="K29" s="2">
-        <v>27003.0</v>
+        <v>16188</v>
       </c>
       <c r="L29" s="2">
-        <v>24012.0</v>
+        <v>6638</v>
       </c>
       <c r="M29" s="2">
-        <v>114049.0</v>
+        <v>114049</v>
       </c>
       <c r="N29" s="2">
-        <v>140420.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>140420</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
-        <v>27064.0</v>
+        <v>27064</v>
       </c>
       <c r="C30" s="2">
-        <v>3907.0</v>
+        <v>3907</v>
       </c>
       <c r="D30" s="2">
-        <v>192755.0</v>
+        <v>192755</v>
       </c>
       <c r="E30" s="2">
-        <v>5080.0</v>
+        <v>5080</v>
       </c>
       <c r="F30" s="2">
-        <v>103662.0</v>
+        <v>103662</v>
       </c>
       <c r="G30" s="2">
-        <v>12369.0</v>
+        <v>12369</v>
       </c>
       <c r="H30" s="2">
-        <v>8652.0</v>
+        <v>8652</v>
       </c>
       <c r="I30" s="2">
-        <v>238239.0</v>
+        <v>238239</v>
       </c>
       <c r="J30" s="2">
-        <v>80220.0</v>
+        <v>80220</v>
       </c>
       <c r="K30" s="2">
-        <v>28675.0</v>
+        <v>16268</v>
       </c>
       <c r="L30" s="2">
-        <v>24139.0</v>
+        <v>6863</v>
       </c>
       <c r="M30" s="2">
-        <v>87131.0</v>
+        <v>87131</v>
       </c>
       <c r="N30" s="2">
-        <v>139410.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>139410</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
-        <v>30852.0</v>
+        <v>30852</v>
       </c>
       <c r="C31" s="2">
-        <v>4192.0</v>
+        <v>4192</v>
       </c>
       <c r="D31" s="2">
-        <v>188818.0</v>
+        <v>188818</v>
       </c>
       <c r="E31" s="2">
-        <v>5245.0</v>
+        <v>5245</v>
       </c>
       <c r="F31" s="2">
-        <v>108828.0</v>
+        <v>108828</v>
       </c>
       <c r="G31" s="2">
-        <v>12513.0</v>
+        <v>12513</v>
       </c>
       <c r="H31" s="2">
-        <v>8956.0</v>
+        <v>8956</v>
       </c>
       <c r="I31" s="2">
-        <v>237714.0</v>
+        <v>237714</v>
       </c>
       <c r="J31" s="2">
-        <v>76167.0</v>
+        <v>76167</v>
       </c>
       <c r="K31" s="2">
-        <v>48463.0</v>
+        <v>15639</v>
       </c>
       <c r="L31" s="2">
-        <v>24038.0</v>
+        <v>6577</v>
       </c>
       <c r="M31" s="2">
-        <v>87708.0</v>
+        <v>87708</v>
       </c>
       <c r="N31" s="2">
-        <v>140638.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>140638</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
-        <v>26891.0</v>
+        <v>26891</v>
       </c>
       <c r="C32" s="2">
-        <v>4262.0</v>
+        <v>4262</v>
       </c>
       <c r="D32" s="2">
-        <v>196460.0</v>
+        <v>196460</v>
       </c>
       <c r="E32" s="2">
-        <v>5278.0</v>
+        <v>5278</v>
       </c>
       <c r="F32" s="2">
-        <v>106830.0</v>
+        <v>106830</v>
       </c>
       <c r="G32" s="2">
-        <v>12566.0</v>
+        <v>12566</v>
       </c>
       <c r="H32" s="2">
-        <v>8718.0</v>
+        <v>8718</v>
       </c>
       <c r="I32" s="2">
-        <v>237692.0</v>
+        <v>237692</v>
       </c>
       <c r="J32" s="2">
-        <v>80004.0</v>
+        <v>80004</v>
       </c>
       <c r="K32" s="2">
-        <v>48650.0</v>
+        <v>15568</v>
       </c>
       <c r="L32" s="2">
-        <v>25018.0</v>
+        <v>7061</v>
       </c>
       <c r="M32" s="2">
-        <v>108679.0</v>
+        <v>108679</v>
       </c>
       <c r="N32" s="2">
-        <v>104916.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>104916</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" ref="B34:N34" si="1">AVERAGE(B3:B32)</f>
-        <v>28637.43333</v>
+        <f t="shared" ref="B34:N34" si="0">AVERAGE(B3:B32)</f>
+        <v>28637.433333333334</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4032.7</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="1"/>
-        <v>130250.4667</v>
+        <f t="shared" si="0"/>
+        <v>130250.46666666666</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="1"/>
-        <v>4956.666667</v>
+        <f t="shared" si="0"/>
+        <v>4956.666666666667</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>122011.9</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="1"/>
-        <v>12886.13333</v>
+        <f t="shared" si="0"/>
+        <v>12886.133333333333</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7918.6</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>330439.2</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" si="1"/>
-        <v>78588.4</v>
+        <f t="shared" si="0"/>
+        <v>78588.399999999994</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="1"/>
-        <v>32836.16667</v>
+        <f t="shared" si="0"/>
+        <v>15977.2</v>
       </c>
       <c r="L34" s="3">
-        <f t="shared" si="1"/>
-        <v>32638.63333</v>
+        <f t="shared" si="0"/>
+        <v>6526.8666666666668</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" si="1"/>
-        <v>106910.0667</v>
+        <f t="shared" si="0"/>
+        <v>106910.06666666667</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>108556.2</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="3">
-        <f t="shared" ref="B35:C35" si="2">B34/100</f>
-        <v>286.3743333</v>
+        <f t="shared" ref="B35:C35" si="1">B34/100</f>
+        <v>286.37433333333337</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="2"/>
-        <v>40.327</v>
+        <f t="shared" si="1"/>
+        <v>40.326999999999998</v>
       </c>
       <c r="D35" s="3">
         <f>D34</f>
-        <v>130250.4667</v>
+        <v>130250.46666666666</v>
       </c>
       <c r="E35" s="3">
         <f>E34/1000000</f>
-        <v>0.004956666667</v>
+        <v>4.9566666666666674E-3</v>
       </c>
       <c r="F35" s="3">
         <f>F34</f>
@@ -1732,38 +1760,38 @@
       </c>
       <c r="G35" s="3">
         <f>G34/10</f>
-        <v>1288.613333</v>
+        <v>1288.6133333333332</v>
       </c>
       <c r="H35" s="3">
         <f>H34/1000</f>
-        <v>7.9186</v>
+        <v>7.9186000000000005</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" ref="I35:J35" si="3">I34</f>
+        <f t="shared" ref="I35:J35" si="2">I34</f>
         <v>330439.2</v>
       </c>
       <c r="J35" s="3">
+        <f t="shared" si="2"/>
+        <v>78588.399999999994</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" ref="K35:L35" si="3">K34/100</f>
+        <v>159.77200000000002</v>
+      </c>
+      <c r="L35" s="3">
         <f t="shared" si="3"/>
-        <v>78588.4</v>
-      </c>
-      <c r="K35" s="3">
-        <f t="shared" ref="K35:L35" si="4">K34/100</f>
-        <v>328.3616667</v>
-      </c>
-      <c r="L35" s="3">
+        <v>65.268666666666661</v>
+      </c>
+      <c r="M35" s="3">
+        <f t="shared" ref="M35:N35" si="4">M34/10</f>
+        <v>10691.006666666666</v>
+      </c>
+      <c r="N35" s="3">
         <f t="shared" si="4"/>
-        <v>326.3863333</v>
-      </c>
-      <c r="M35" s="3">
-        <f t="shared" ref="M35:N35" si="5">M34/10</f>
-        <v>10691.00667</v>
-      </c>
-      <c r="N35" s="3">
-        <f t="shared" si="5"/>
-        <v>10855.62</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>10855.619999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>13</v>
       </c>
@@ -1771,137 +1799,147 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" ref="B38:C38" si="6">B35</f>
-        <v>286.3743333</v>
+        <f t="shared" ref="B38:C38" si="5">B35</f>
+        <v>286.37433333333337</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="6"/>
-        <v>40.327</v>
-      </c>
-    </row>
-    <row r="39">
+        <f t="shared" si="5"/>
+        <v>40.326999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="3">
         <f>D35</f>
-        <v>130250.4667</v>
+        <v>130250.46666666666</v>
       </c>
       <c r="C39" s="3">
         <f>F35</f>
         <v>122011.9</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="3">
-        <f t="shared" ref="B40:C40" si="7">G35</f>
-        <v>1288.613333</v>
+        <f t="shared" ref="B40:C40" si="6">G35</f>
+        <v>1288.6133333333332</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="7"/>
-        <v>7.9186</v>
-      </c>
-    </row>
-    <row r="41">
+        <f t="shared" si="6"/>
+        <v>7.9186000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="3">
-        <f t="shared" ref="B41:C41" si="8">I35</f>
+        <f t="shared" ref="B41:C41" si="7">I35</f>
         <v>330439.2</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="8"/>
-        <v>78588.4</v>
-      </c>
-    </row>
-    <row r="42">
+        <f t="shared" si="7"/>
+        <v>78588.399999999994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="3">
-        <f t="shared" ref="B42:C42" si="9">K35</f>
-        <v>328.3616667</v>
+        <f t="shared" ref="B42:C42" si="8">K35</f>
+        <v>159.77200000000002</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="9"/>
-        <v>326.3863333</v>
-      </c>
-    </row>
-    <row r="43">
+        <f t="shared" si="8"/>
+        <v>65.268666666666661</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="3">
-        <f t="shared" ref="B43:C43" si="10">M35</f>
-        <v>10691.00667</v>
+        <f t="shared" ref="B43:C43" si="9">M35</f>
+        <v>10691.006666666666</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="10"/>
-        <v>10855.62</v>
+        <f t="shared" si="9"/>
+        <v>10855.619999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="16.63"/>
-    <col customWidth="1" min="5" max="5" width="49.63"/>
-    <col customWidth="1" min="6" max="6" width="28.63"/>
-    <col customWidth="1" min="8" max="8" width="17.5"/>
-    <col customWidth="1" min="9" max="9" width="13.75"/>
-    <col customWidth="1" min="12" max="12" width="18.0"/>
-    <col customWidth="1" min="14" max="14" width="18.5"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="5"/>
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1933,7 +1971,7 @@
         <v>6</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>11</v>
@@ -1942,7 +1980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3">
         <f>Measurements!B3/100</f>
         <v>191.53</v>
@@ -1957,7 +1995,7 @@
       </c>
       <c r="E3" s="3">
         <f>Measurements!E3/1000000</f>
-        <v>0.004937</v>
+        <v>4.9370000000000004E-3</v>
       </c>
       <c r="F3" s="3">
         <f>Measurements!F3</f>
@@ -1969,7 +2007,7 @@
       </c>
       <c r="H3" s="3">
         <f>Measurements!H3/1000</f>
-        <v>7.454</v>
+        <v>7.4539999999999997</v>
       </c>
       <c r="I3" s="3">
         <f>Measurements!I3</f>
@@ -1981,11 +2019,11 @@
       </c>
       <c r="K3" s="3">
         <f>Measurements!K3/100</f>
-        <v>302.11</v>
+        <v>157.03</v>
       </c>
       <c r="L3" s="3">
-        <f>Measurements!L3/100</f>
-        <v>263.56</v>
+        <f>Measurements!L3/1000</f>
+        <v>6.2</v>
       </c>
       <c r="M3" s="3">
         <f>Measurements!M3/10</f>
@@ -1993,17 +2031,17 @@
       </c>
       <c r="N3" s="3">
         <f>Measurements!N3/10</f>
-        <v>9673.3</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>9673.2999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3">
         <f>Measurements!B4/100</f>
         <v>202.05</v>
       </c>
       <c r="C4" s="3">
         <f>Measurements!C4/100</f>
-        <v>35.91</v>
+        <v>35.909999999999997</v>
       </c>
       <c r="D4" s="3">
         <f>Measurements!D4</f>
@@ -2011,7 +2049,7 @@
       </c>
       <c r="E4" s="3">
         <f>Measurements!E4/1000000</f>
-        <v>0.004799</v>
+        <v>4.7990000000000003E-3</v>
       </c>
       <c r="F4" s="3">
         <f>Measurements!F4</f>
@@ -2035,11 +2073,11 @@
       </c>
       <c r="K4" s="3">
         <f>Measurements!K4/100</f>
-        <v>322.76</v>
+        <v>148.72999999999999</v>
       </c>
       <c r="L4" s="3">
-        <f>Measurements!L4/100</f>
-        <v>254.27</v>
+        <f>Measurements!L4/1000</f>
+        <v>5.7409999999999997</v>
       </c>
       <c r="M4" s="3">
         <f>Measurements!M4/10</f>
@@ -2047,13 +2085,13 @@
       </c>
       <c r="N4" s="3">
         <f>Measurements!N4/10</f>
-        <v>8733.8</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>8733.7999999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <f>Measurements!B5/100</f>
-        <v>300.21</v>
+        <v>300.20999999999998</v>
       </c>
       <c r="C5" s="3">
         <f>Measurements!C5/100</f>
@@ -2065,7 +2103,7 @@
       </c>
       <c r="E5" s="3">
         <f>Measurements!E5/1000000</f>
-        <v>0.004703</v>
+        <v>4.7029999999999997E-3</v>
       </c>
       <c r="F5" s="3">
         <f>Measurements!F5</f>
@@ -2077,7 +2115,7 @@
       </c>
       <c r="H5" s="3">
         <f>Measurements!H5/1000</f>
-        <v>5.437</v>
+        <v>5.4370000000000003</v>
       </c>
       <c r="I5" s="3">
         <f>Measurements!I5</f>
@@ -2089,11 +2127,11 @@
       </c>
       <c r="K5" s="3">
         <f>Measurements!K5/100</f>
-        <v>291.53</v>
+        <v>165.05</v>
       </c>
       <c r="L5" s="3">
-        <f>Measurements!L5/100</f>
-        <v>413.54</v>
+        <f>Measurements!L5/1000</f>
+        <v>6.383</v>
       </c>
       <c r="M5" s="3">
         <f>Measurements!M5/10</f>
@@ -2104,7 +2142,7 @@
         <v>8316.4</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <f>Measurements!B6/100</f>
         <v>299.36</v>
@@ -2119,7 +2157,7 @@
       </c>
       <c r="E6" s="3">
         <f>Measurements!E6/1000000</f>
-        <v>0.004948</v>
+        <v>4.9480000000000001E-3</v>
       </c>
       <c r="F6" s="3">
         <f>Measurements!F6</f>
@@ -2143,11 +2181,11 @@
       </c>
       <c r="K6" s="3">
         <f>Measurements!K6/100</f>
-        <v>271.97</v>
+        <v>146.47999999999999</v>
       </c>
       <c r="L6" s="3">
-        <f>Measurements!L6/100</f>
-        <v>496.74</v>
+        <f>Measurements!L6/1000</f>
+        <v>6.758</v>
       </c>
       <c r="M6" s="3">
         <f>Measurements!M6/10</f>
@@ -2158,7 +2196,7 @@
         <v>8616.4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <f>Measurements!B7/100</f>
         <v>319.83</v>
@@ -2173,7 +2211,7 @@
       </c>
       <c r="E7" s="3">
         <f>Measurements!E7/1000000</f>
-        <v>0.004907</v>
+        <v>4.9069999999999999E-3</v>
       </c>
       <c r="F7" s="3">
         <f>Measurements!F7</f>
@@ -2185,7 +2223,7 @@
       </c>
       <c r="H7" s="3">
         <f>Measurements!H7/1000</f>
-        <v>5.689</v>
+        <v>5.6890000000000001</v>
       </c>
       <c r="I7" s="3">
         <f>Measurements!I7</f>
@@ -2197,11 +2235,11 @@
       </c>
       <c r="K7" s="3">
         <f>Measurements!K7/100</f>
-        <v>272.43</v>
+        <v>152.09</v>
       </c>
       <c r="L7" s="3">
-        <f>Measurements!L7/100</f>
-        <v>467.45</v>
+        <f>Measurements!L7/1000</f>
+        <v>6.0279999999999996</v>
       </c>
       <c r="M7" s="3">
         <f>Measurements!M7/10</f>
@@ -2212,14 +2250,14 @@
         <v>13900.7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
         <f>Measurements!B8/100</f>
         <v>284.62</v>
       </c>
       <c r="C8" s="3">
         <f>Measurements!C8/100</f>
-        <v>34.77</v>
+        <v>34.770000000000003</v>
       </c>
       <c r="D8" s="3">
         <f>Measurements!D8</f>
@@ -2227,7 +2265,7 @@
       </c>
       <c r="E8" s="3">
         <f>Measurements!E8/1000000</f>
-        <v>0.005128</v>
+        <v>5.1279999999999997E-3</v>
       </c>
       <c r="F8" s="3">
         <f>Measurements!F8</f>
@@ -2239,7 +2277,7 @@
       </c>
       <c r="H8" s="3">
         <f>Measurements!H8/1000</f>
-        <v>7.347</v>
+        <v>7.3470000000000004</v>
       </c>
       <c r="I8" s="3">
         <f>Measurements!I8</f>
@@ -2251,11 +2289,11 @@
       </c>
       <c r="K8" s="3">
         <f>Measurements!K8/100</f>
-        <v>396.35</v>
+        <v>148.91</v>
       </c>
       <c r="L8" s="3">
-        <f>Measurements!L8/100</f>
-        <v>455.35</v>
+        <f>Measurements!L8/1000</f>
+        <v>5.0289999999999999</v>
       </c>
       <c r="M8" s="3">
         <f>Measurements!M8/10</f>
@@ -2266,7 +2304,7 @@
         <v>14281.6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3">
         <f>Measurements!B9/100</f>
         <v>302</v>
@@ -2281,7 +2319,7 @@
       </c>
       <c r="E9" s="3">
         <f>Measurements!E9/1000000</f>
-        <v>0.005278</v>
+        <v>5.2779999999999997E-3</v>
       </c>
       <c r="F9" s="3">
         <f>Measurements!F9</f>
@@ -2289,11 +2327,11 @@
       </c>
       <c r="G9" s="3">
         <f>Measurements!G9/10</f>
-        <v>1272.1</v>
+        <v>1272.0999999999999</v>
       </c>
       <c r="H9" s="3">
         <f>Measurements!H9/1000</f>
-        <v>8.228</v>
+        <v>8.2279999999999998</v>
       </c>
       <c r="I9" s="3">
         <f>Measurements!I9</f>
@@ -2305,11 +2343,11 @@
       </c>
       <c r="K9" s="3">
         <f>Measurements!K9/100</f>
-        <v>462.14</v>
+        <v>169.38</v>
       </c>
       <c r="L9" s="3">
-        <f>Measurements!L9/100</f>
-        <v>452.69</v>
+        <f>Measurements!L9/1000</f>
+        <v>5.2329999999999997</v>
       </c>
       <c r="M9" s="3">
         <f>Measurements!M9/10</f>
@@ -2320,7 +2358,7 @@
         <v>13648.9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3">
         <f>Measurements!B10/100</f>
         <v>318.69</v>
@@ -2335,7 +2373,7 @@
       </c>
       <c r="E10" s="3">
         <f>Measurements!E10/1000000</f>
-        <v>0.005023</v>
+        <v>5.0229999999999997E-3</v>
       </c>
       <c r="F10" s="3">
         <f>Measurements!F10</f>
@@ -2347,7 +2385,7 @@
       </c>
       <c r="H10" s="3">
         <f>Measurements!H10/1000</f>
-        <v>8.001</v>
+        <v>8.0009999999999994</v>
       </c>
       <c r="I10" s="3">
         <f>Measurements!I10</f>
@@ -2359,29 +2397,29 @@
       </c>
       <c r="K10" s="3">
         <f>Measurements!K10/100</f>
-        <v>453.54</v>
+        <v>208.85</v>
       </c>
       <c r="L10" s="3">
-        <f>Measurements!L10/100</f>
-        <v>466.16</v>
+        <f>Measurements!L10/1000</f>
+        <v>5.6319999999999997</v>
       </c>
       <c r="M10" s="3">
         <f>Measurements!M10/10</f>
-        <v>9266.8</v>
+        <v>9266.7999999999993</v>
       </c>
       <c r="N10" s="3">
         <f>Measurements!N10/10</f>
         <v>7398.8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3">
         <f>Measurements!B11/100</f>
         <v>311.13</v>
       </c>
       <c r="C11" s="3">
         <f>Measurements!C11/100</f>
-        <v>38.27</v>
+        <v>38.270000000000003</v>
       </c>
       <c r="D11" s="3">
         <f>Measurements!D11</f>
@@ -2389,7 +2427,7 @@
       </c>
       <c r="E11" s="3">
         <f>Measurements!E11/1000000</f>
-        <v>0.004857</v>
+        <v>4.8570000000000002E-3</v>
       </c>
       <c r="F11" s="3">
         <f>Measurements!F11</f>
@@ -2397,11 +2435,11 @@
       </c>
       <c r="G11" s="3">
         <f>Measurements!G11/10</f>
-        <v>1294.9</v>
+        <v>1294.9000000000001</v>
       </c>
       <c r="H11" s="3">
         <f>Measurements!H11/1000</f>
-        <v>8.026</v>
+        <v>8.0259999999999998</v>
       </c>
       <c r="I11" s="3">
         <f>Measurements!I11</f>
@@ -2413,22 +2451,22 @@
       </c>
       <c r="K11" s="3">
         <f>Measurements!K11/100</f>
-        <v>483.96</v>
+        <v>197.95</v>
       </c>
       <c r="L11" s="3">
-        <f>Measurements!L11/100</f>
-        <v>488.8</v>
+        <f>Measurements!L11/1000</f>
+        <v>6.7069999999999999</v>
       </c>
       <c r="M11" s="3">
         <f>Measurements!M11/10</f>
-        <v>8760.8</v>
+        <v>8760.7999999999993</v>
       </c>
       <c r="N11" s="3">
         <f>Measurements!N11/10</f>
         <v>8756</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
         <f>Measurements!B12/100</f>
         <v>309.73</v>
@@ -2443,7 +2481,7 @@
       </c>
       <c r="E12" s="3">
         <f>Measurements!E12/1000000</f>
-        <v>0.004739</v>
+        <v>4.7390000000000002E-3</v>
       </c>
       <c r="F12" s="3">
         <f>Measurements!F12</f>
@@ -2467,25 +2505,25 @@
       </c>
       <c r="K12" s="3">
         <f>Measurements!K12/100</f>
-        <v>471.55</v>
+        <v>175.25</v>
       </c>
       <c r="L12" s="3">
-        <f>Measurements!L12/100</f>
-        <v>467.49</v>
+        <f>Measurements!L12/1000</f>
+        <v>6.7910000000000004</v>
       </c>
       <c r="M12" s="3">
         <f>Measurements!M12/10</f>
-        <v>8466.7</v>
+        <v>8466.7000000000007</v>
       </c>
       <c r="N12" s="3">
         <f>Measurements!N12/10</f>
-        <v>8567.3</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>8567.2999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3">
         <f>Measurements!B13/100</f>
-        <v>304.53</v>
+        <v>304.52999999999997</v>
       </c>
       <c r="C13" s="3">
         <f>Measurements!C13/100</f>
@@ -2497,7 +2535,7 @@
       </c>
       <c r="E13" s="3">
         <f>Measurements!E13/1000000</f>
-        <v>0.004958</v>
+        <v>4.9579999999999997E-3</v>
       </c>
       <c r="F13" s="3">
         <f>Measurements!F13</f>
@@ -2509,7 +2547,7 @@
       </c>
       <c r="H13" s="3">
         <f>Measurements!H13/1000</f>
-        <v>7.904</v>
+        <v>7.9039999999999999</v>
       </c>
       <c r="I13" s="3">
         <f>Measurements!I13</f>
@@ -2521,29 +2559,29 @@
       </c>
       <c r="K13" s="3">
         <f>Measurements!K13/100</f>
-        <v>337.49</v>
+        <v>162.01</v>
       </c>
       <c r="L13" s="3">
-        <f>Measurements!L13/100</f>
-        <v>294.23</v>
+        <f>Measurements!L13/1000</f>
+        <v>6.8390000000000004</v>
       </c>
       <c r="M13" s="3">
         <f>Measurements!M13/10</f>
-        <v>9056.8</v>
+        <v>9056.7999999999993</v>
       </c>
       <c r="N13" s="3">
         <f>Measurements!N13/10</f>
         <v>7965.6</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3">
         <f>Measurements!B14/100</f>
         <v>307.36</v>
       </c>
       <c r="C14" s="3">
         <f>Measurements!C14/100</f>
-        <v>34.98</v>
+        <v>34.979999999999997</v>
       </c>
       <c r="D14" s="3">
         <f>Measurements!D14</f>
@@ -2551,7 +2589,7 @@
       </c>
       <c r="E14" s="3">
         <f>Measurements!E14/1000000</f>
-        <v>0.00497</v>
+        <v>4.9699999999999996E-3</v>
       </c>
       <c r="F14" s="3">
         <f>Measurements!F14</f>
@@ -2559,11 +2597,11 @@
       </c>
       <c r="G14" s="3">
         <f>Measurements!G14/10</f>
-        <v>1259.6</v>
+        <v>1259.5999999999999</v>
       </c>
       <c r="H14" s="3">
         <f>Measurements!H14/1000</f>
-        <v>8.118</v>
+        <v>8.1180000000000003</v>
       </c>
       <c r="I14" s="3">
         <f>Measurements!I14</f>
@@ -2575,11 +2613,11 @@
       </c>
       <c r="K14" s="3">
         <f>Measurements!K14/100</f>
-        <v>315.41</v>
+        <v>147.05000000000001</v>
       </c>
       <c r="L14" s="3">
-        <f>Measurements!L14/100</f>
-        <v>307.01</v>
+        <f>Measurements!L14/1000</f>
+        <v>6.6029999999999998</v>
       </c>
       <c r="M14" s="3">
         <f>Measurements!M14/10</f>
@@ -2590,10 +2628,10 @@
         <v>8714.1</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3">
         <f>Measurements!B15/100</f>
-        <v>308.84</v>
+        <v>308.83999999999997</v>
       </c>
       <c r="C15" s="3">
         <f>Measurements!C15/100</f>
@@ -2605,7 +2643,7 @@
       </c>
       <c r="E15" s="3">
         <f>Measurements!E15/1000000</f>
-        <v>0.004783</v>
+        <v>4.7829999999999999E-3</v>
       </c>
       <c r="F15" s="3">
         <f>Measurements!F15</f>
@@ -2629,11 +2667,11 @@
       </c>
       <c r="K15" s="3">
         <f>Measurements!K15/100</f>
-        <v>319.88</v>
+        <v>146.03</v>
       </c>
       <c r="L15" s="3">
-        <f>Measurements!L15/100</f>
-        <v>312.87</v>
+        <f>Measurements!L15/1000</f>
+        <v>6.5430000000000001</v>
       </c>
       <c r="M15" s="3">
         <f>Measurements!M15/10</f>
@@ -2644,7 +2682,7 @@
         <v>10371</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3">
         <f>Measurements!B16/100</f>
         <v>285.39</v>
@@ -2659,7 +2697,7 @@
       </c>
       <c r="E16" s="3">
         <f>Measurements!E16/1000000</f>
-        <v>0.004643</v>
+        <v>4.6430000000000004E-3</v>
       </c>
       <c r="F16" s="3">
         <f>Measurements!F16</f>
@@ -2667,11 +2705,11 @@
       </c>
       <c r="G16" s="3">
         <f>Measurements!G16/10</f>
-        <v>1264.4</v>
+        <v>1264.4000000000001</v>
       </c>
       <c r="H16" s="3">
         <f>Measurements!H16/1000</f>
-        <v>8.175</v>
+        <v>8.1750000000000007</v>
       </c>
       <c r="I16" s="3">
         <f>Measurements!I16</f>
@@ -2683,22 +2721,22 @@
       </c>
       <c r="K16" s="3">
         <f>Measurements!K16/100</f>
-        <v>320.92</v>
+        <v>147.19</v>
       </c>
       <c r="L16" s="3">
-        <f>Measurements!L16/100</f>
-        <v>316.62</v>
+        <f>Measurements!L16/1000</f>
+        <v>6.5270000000000001</v>
       </c>
       <c r="M16" s="3">
         <f>Measurements!M16/10</f>
-        <v>9380.7</v>
+        <v>9380.7000000000007</v>
       </c>
       <c r="N16" s="3">
         <f>Measurements!N16/10</f>
         <v>9692</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3">
         <f>Measurements!B17/100</f>
         <v>244.56</v>
@@ -2713,7 +2751,7 @@
       </c>
       <c r="E17" s="3">
         <f>Measurements!E17/1000000</f>
-        <v>0.005202</v>
+        <v>5.202E-3</v>
       </c>
       <c r="F17" s="3">
         <f>Measurements!F17</f>
@@ -2725,7 +2763,7 @@
       </c>
       <c r="H17" s="3">
         <f>Measurements!H17/1000</f>
-        <v>8.339</v>
+        <v>8.3390000000000004</v>
       </c>
       <c r="I17" s="3">
         <f>Measurements!I17</f>
@@ -2737,11 +2775,11 @@
       </c>
       <c r="K17" s="3">
         <f>Measurements!K17/100</f>
-        <v>288.21</v>
+        <v>147.12</v>
       </c>
       <c r="L17" s="3">
-        <f>Measurements!L17/100</f>
-        <v>305.57</v>
+        <f>Measurements!L17/1000</f>
+        <v>7.0270000000000001</v>
       </c>
       <c r="M17" s="3">
         <f>Measurements!M17/10</f>
@@ -2752,7 +2790,7 @@
         <v>9346.6</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3">
         <f>Measurements!B18/100</f>
         <v>281.76</v>
@@ -2767,7 +2805,7 @@
       </c>
       <c r="E18" s="3">
         <f>Measurements!E18/1000000</f>
-        <v>0.005179</v>
+        <v>5.1789999999999996E-3</v>
       </c>
       <c r="F18" s="3">
         <f>Measurements!F18</f>
@@ -2779,7 +2817,7 @@
       </c>
       <c r="H18" s="3">
         <f>Measurements!H18/1000</f>
-        <v>8.275</v>
+        <v>8.2750000000000004</v>
       </c>
       <c r="I18" s="3">
         <f>Measurements!I18</f>
@@ -2791,11 +2829,11 @@
       </c>
       <c r="K18" s="3">
         <f>Measurements!K18/100</f>
-        <v>271.74</v>
+        <v>149.44999999999999</v>
       </c>
       <c r="L18" s="3">
-        <f>Measurements!L18/100</f>
-        <v>312.38</v>
+        <f>Measurements!L18/1000</f>
+        <v>6.7389999999999999</v>
       </c>
       <c r="M18" s="3">
         <f>Measurements!M18/10</f>
@@ -2806,10 +2844,10 @@
         <v>11405.4</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <f>Measurements!B19/100</f>
-        <v>294.28</v>
+        <v>294.27999999999997</v>
       </c>
       <c r="C19" s="3">
         <f>Measurements!C19/100</f>
@@ -2821,7 +2859,7 @@
       </c>
       <c r="E19" s="3">
         <f>Measurements!E19/1000000</f>
-        <v>0.004948</v>
+        <v>4.9480000000000001E-3</v>
       </c>
       <c r="F19" s="3">
         <f>Measurements!F19</f>
@@ -2845,11 +2883,11 @@
       </c>
       <c r="K19" s="3">
         <f>Measurements!K19/100</f>
-        <v>271.46</v>
+        <v>157.61000000000001</v>
       </c>
       <c r="L19" s="3">
-        <f>Measurements!L19/100</f>
-        <v>317.26</v>
+        <f>Measurements!L19/1000</f>
+        <v>6.9509999999999996</v>
       </c>
       <c r="M19" s="3">
         <f>Measurements!M19/10</f>
@@ -2860,7 +2898,7 @@
         <v>14454.9</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <f>Measurements!B20/100</f>
         <v>316.8</v>
@@ -2875,7 +2913,7 @@
       </c>
       <c r="E20" s="3">
         <f>Measurements!E20/1000000</f>
-        <v>0.004992</v>
+        <v>4.9919999999999999E-3</v>
       </c>
       <c r="F20" s="3">
         <f>Measurements!F20</f>
@@ -2887,7 +2925,7 @@
       </c>
       <c r="H20" s="3">
         <f>Measurements!H20/1000</f>
-        <v>8.956</v>
+        <v>8.9559999999999995</v>
       </c>
       <c r="I20" s="3">
         <f>Measurements!I20</f>
@@ -2899,22 +2937,22 @@
       </c>
       <c r="K20" s="3">
         <f>Measurements!K20/100</f>
-        <v>271.58</v>
+        <v>158.63999999999999</v>
       </c>
       <c r="L20" s="3">
-        <f>Measurements!L20/100</f>
-        <v>305.93</v>
+        <f>Measurements!L20/1000</f>
+        <v>6.7210000000000001</v>
       </c>
       <c r="M20" s="3">
         <f>Measurements!M20/10</f>
-        <v>8811.3</v>
+        <v>8811.2999999999993</v>
       </c>
       <c r="N20" s="3">
         <f>Measurements!N20/10</f>
         <v>14132.9</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3">
         <f>Measurements!B21/100</f>
         <v>301.75</v>
@@ -2929,7 +2967,7 @@
       </c>
       <c r="E21" s="3">
         <f>Measurements!E21/1000000</f>
-        <v>0.00492</v>
+        <v>4.9199999999999999E-3</v>
       </c>
       <c r="F21" s="3">
         <f>Measurements!F21</f>
@@ -2941,7 +2979,7 @@
       </c>
       <c r="H21" s="3">
         <f>Measurements!H21/1000</f>
-        <v>8.289</v>
+        <v>8.2889999999999997</v>
       </c>
       <c r="I21" s="3">
         <f>Measurements!I21</f>
@@ -2953,11 +2991,11 @@
       </c>
       <c r="K21" s="3">
         <f>Measurements!K21/100</f>
-        <v>271.5</v>
+        <v>159.21</v>
       </c>
       <c r="L21" s="3">
-        <f>Measurements!L21/100</f>
-        <v>298.99</v>
+        <f>Measurements!L21/1000</f>
+        <v>6.9960000000000004</v>
       </c>
       <c r="M21" s="3">
         <f>Measurements!M21/10</f>
@@ -2968,7 +3006,7 @@
         <v>12224.5</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3">
         <f>Measurements!B22/100</f>
         <v>293.99</v>
@@ -2983,7 +3021,7 @@
       </c>
       <c r="E22" s="3">
         <f>Measurements!E22/1000000</f>
-        <v>0.004968</v>
+        <v>4.9680000000000002E-3</v>
       </c>
       <c r="F22" s="3">
         <f>Measurements!F22</f>
@@ -2991,11 +3029,11 @@
       </c>
       <c r="G22" s="3">
         <f>Measurements!G22/10</f>
-        <v>1301.6</v>
+        <v>1301.5999999999999</v>
       </c>
       <c r="H22" s="3">
         <f>Measurements!H22/1000</f>
-        <v>8.329</v>
+        <v>8.3290000000000006</v>
       </c>
       <c r="I22" s="3">
         <f>Measurements!I22</f>
@@ -3007,11 +3045,11 @@
       </c>
       <c r="K22" s="3">
         <f>Measurements!K22/100</f>
-        <v>270.22</v>
+        <v>156.13</v>
       </c>
       <c r="L22" s="3">
-        <f>Measurements!L22/100</f>
-        <v>301.03</v>
+        <f>Measurements!L22/1000</f>
+        <v>6.9059999999999997</v>
       </c>
       <c r="M22" s="3">
         <f>Measurements!M22/10</f>
@@ -3022,10 +3060,10 @@
         <v>7487.6</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3">
         <f>Measurements!B23/100</f>
-        <v>292.47</v>
+        <v>292.47000000000003</v>
       </c>
       <c r="C23" s="3">
         <f>Measurements!C23/100</f>
@@ -3037,7 +3075,7 @@
       </c>
       <c r="E23" s="3">
         <f>Measurements!E23/1000000</f>
-        <v>0.00479</v>
+        <v>4.79E-3</v>
       </c>
       <c r="F23" s="3">
         <f>Measurements!F23</f>
@@ -3061,11 +3099,11 @@
       </c>
       <c r="K23" s="3">
         <f>Measurements!K23/100</f>
-        <v>269.86</v>
+        <v>159.28</v>
       </c>
       <c r="L23" s="3">
-        <f>Measurements!L23/100</f>
-        <v>277.4</v>
+        <f>Measurements!L23/1000</f>
+        <v>6.89</v>
       </c>
       <c r="M23" s="3">
         <f>Measurements!M23/10</f>
@@ -3076,7 +3114,7 @@
         <v>7925.3</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3">
         <f>Measurements!B24/100</f>
         <v>288.45</v>
@@ -3091,7 +3129,7 @@
       </c>
       <c r="E24" s="3">
         <f>Measurements!E24/1000000</f>
-        <v>0.004895</v>
+        <v>4.895E-3</v>
       </c>
       <c r="F24" s="3">
         <f>Measurements!F24</f>
@@ -3099,11 +3137,11 @@
       </c>
       <c r="G24" s="3">
         <f>Measurements!G24/10</f>
-        <v>1294.9</v>
+        <v>1294.9000000000001</v>
       </c>
       <c r="H24" s="3">
         <f>Measurements!H24/1000</f>
-        <v>8.517</v>
+        <v>8.5169999999999995</v>
       </c>
       <c r="I24" s="3">
         <f>Measurements!I24</f>
@@ -3115,11 +3153,11 @@
       </c>
       <c r="K24" s="3">
         <f>Measurements!K24/100</f>
-        <v>273.02</v>
+        <v>157.41</v>
       </c>
       <c r="L24" s="3">
-        <f>Measurements!L24/100</f>
-        <v>247.31</v>
+        <f>Measurements!L24/1000</f>
+        <v>6.569</v>
       </c>
       <c r="M24" s="3">
         <f>Measurements!M24/10</f>
@@ -3127,10 +3165,10 @@
       </c>
       <c r="N24" s="3">
         <f>Measurements!N24/10</f>
-        <v>9550.3</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>9550.2999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B25" s="3">
         <f>Measurements!B25/100</f>
         <v>300.48</v>
@@ -3145,7 +3183,7 @@
       </c>
       <c r="E25" s="3">
         <f>Measurements!E25/1000000</f>
-        <v>0.004878</v>
+        <v>4.8780000000000004E-3</v>
       </c>
       <c r="F25" s="3">
         <f>Measurements!F25</f>
@@ -3153,11 +3191,11 @@
       </c>
       <c r="G25" s="3">
         <f>Measurements!G25/10</f>
-        <v>1276.6</v>
+        <v>1276.5999999999999</v>
       </c>
       <c r="H25" s="3">
         <f>Measurements!H25/1000</f>
-        <v>8.424</v>
+        <v>8.4239999999999995</v>
       </c>
       <c r="I25" s="3">
         <f>Measurements!I25</f>
@@ -3169,25 +3207,25 @@
       </c>
       <c r="K25" s="3">
         <f>Measurements!K25/100</f>
-        <v>276.56</v>
+        <v>157.53</v>
       </c>
       <c r="L25" s="3">
-        <f>Measurements!L25/100</f>
-        <v>240.73</v>
+        <f>Measurements!L25/1000</f>
+        <v>6.5039999999999996</v>
       </c>
       <c r="M25" s="3">
         <f>Measurements!M25/10</f>
-        <v>9408.2</v>
+        <v>9408.2000000000007</v>
       </c>
       <c r="N25" s="3">
         <f>Measurements!N25/10</f>
         <v>14058.1</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="3">
         <f>Measurements!B26/100</f>
-        <v>293.54</v>
+        <v>293.54000000000002</v>
       </c>
       <c r="C26" s="3">
         <f>Measurements!C26/100</f>
@@ -3199,7 +3237,7 @@
       </c>
       <c r="E26" s="3">
         <f>Measurements!E26/1000000</f>
-        <v>0.005114</v>
+        <v>5.1139999999999996E-3</v>
       </c>
       <c r="F26" s="3">
         <f>Measurements!F26</f>
@@ -3207,7 +3245,7 @@
       </c>
       <c r="G26" s="3">
         <f>Measurements!G26/10</f>
-        <v>1261.6</v>
+        <v>1261.5999999999999</v>
       </c>
       <c r="H26" s="3">
         <f>Measurements!H26/1000</f>
@@ -3223,11 +3261,11 @@
       </c>
       <c r="K26" s="3">
         <f>Measurements!K26/100</f>
-        <v>278.12</v>
+        <v>158.55000000000001</v>
       </c>
       <c r="L26" s="3">
-        <f>Measurements!L26/100</f>
-        <v>242.44</v>
+        <f>Measurements!L26/1000</f>
+        <v>6.8949999999999996</v>
       </c>
       <c r="M26" s="3">
         <f>Measurements!M26/10</f>
@@ -3238,7 +3276,7 @@
         <v>11942.4</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="3">
         <f>Measurements!B27/100</f>
         <v>297.69</v>
@@ -3253,7 +3291,7 @@
       </c>
       <c r="E27" s="3">
         <f>Measurements!E27/1000000</f>
-        <v>0.004932</v>
+        <v>4.9319999999999998E-3</v>
       </c>
       <c r="F27" s="3">
         <f>Measurements!F27</f>
@@ -3265,7 +3303,7 @@
       </c>
       <c r="H27" s="3">
         <f>Measurements!H27/1000</f>
-        <v>8.482</v>
+        <v>8.4819999999999993</v>
       </c>
       <c r="I27" s="3">
         <f>Measurements!I27</f>
@@ -3277,11 +3315,11 @@
       </c>
       <c r="K27" s="3">
         <f>Measurements!K27/100</f>
-        <v>288.15</v>
+        <v>161.13999999999999</v>
       </c>
       <c r="L27" s="3">
-        <f>Measurements!L27/100</f>
-        <v>252.63</v>
+        <f>Measurements!L27/1000</f>
+        <v>6.8090000000000002</v>
       </c>
       <c r="M27" s="3">
         <f>Measurements!M27/10</f>
@@ -3292,7 +3330,7 @@
         <v>13345.8</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="3">
         <f>Measurements!B28/100</f>
         <v>279.25</v>
@@ -3307,7 +3345,7 @@
       </c>
       <c r="E28" s="3">
         <f>Measurements!E28/1000000</f>
-        <v>0.004778</v>
+        <v>4.7780000000000001E-3</v>
       </c>
       <c r="F28" s="3">
         <f>Measurements!F28</f>
@@ -3319,7 +3357,7 @@
       </c>
       <c r="H28" s="3">
         <f>Measurements!H28/1000</f>
-        <v>8.847</v>
+        <v>8.8469999999999995</v>
       </c>
       <c r="I28" s="3">
         <f>Measurements!I28</f>
@@ -3331,22 +3369,22 @@
       </c>
       <c r="K28" s="3">
         <f>Measurements!K28/100</f>
-        <v>270.48</v>
+        <v>162.46</v>
       </c>
       <c r="L28" s="3">
-        <f>Measurements!L28/100</f>
-        <v>261.07</v>
+        <f>Measurements!L28/1000</f>
+        <v>6.6459999999999999</v>
       </c>
       <c r="M28" s="3">
         <f>Measurements!M28/10</f>
-        <v>8576.2</v>
+        <v>8576.2000000000007</v>
       </c>
       <c r="N28" s="3">
         <f>Measurements!N28/10</f>
         <v>8620.5</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B29" s="3">
         <f>Measurements!B29/100</f>
         <v>212.87</v>
@@ -3361,7 +3399,7 @@
       </c>
       <c r="E29" s="3">
         <f>Measurements!E29/1000000</f>
-        <v>0.004828</v>
+        <v>4.8279999999999998E-3</v>
       </c>
       <c r="F29" s="3">
         <f>Measurements!F29</f>
@@ -3373,7 +3411,7 @@
       </c>
       <c r="H29" s="3">
         <f>Measurements!H29/1000</f>
-        <v>8.158</v>
+        <v>8.1579999999999995</v>
       </c>
       <c r="I29" s="3">
         <f>Measurements!I29</f>
@@ -3385,11 +3423,11 @@
       </c>
       <c r="K29" s="3">
         <f>Measurements!K29/100</f>
-        <v>270.03</v>
+        <v>161.88</v>
       </c>
       <c r="L29" s="3">
-        <f>Measurements!L29/100</f>
-        <v>240.12</v>
+        <f>Measurements!L29/1000</f>
+        <v>6.6379999999999999</v>
       </c>
       <c r="M29" s="3">
         <f>Measurements!M29/10</f>
@@ -3400,7 +3438,7 @@
         <v>14042</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="3">
         <f>Measurements!B30/100</f>
         <v>270.64</v>
@@ -3415,7 +3453,7 @@
       </c>
       <c r="E30" s="3">
         <f>Measurements!E30/1000000</f>
-        <v>0.00508</v>
+        <v>5.0800000000000003E-3</v>
       </c>
       <c r="F30" s="3">
         <f>Measurements!F30</f>
@@ -3423,11 +3461,11 @@
       </c>
       <c r="G30" s="3">
         <f>Measurements!G30/10</f>
-        <v>1236.9</v>
+        <v>1236.9000000000001</v>
       </c>
       <c r="H30" s="3">
         <f>Measurements!H30/1000</f>
-        <v>8.652</v>
+        <v>8.6519999999999992</v>
       </c>
       <c r="I30" s="3">
         <f>Measurements!I30</f>
@@ -3439,11 +3477,11 @@
       </c>
       <c r="K30" s="3">
         <f>Measurements!K30/100</f>
-        <v>286.75</v>
+        <v>162.68</v>
       </c>
       <c r="L30" s="3">
-        <f>Measurements!L30/100</f>
-        <v>241.39</v>
+        <f>Measurements!L30/1000</f>
+        <v>6.8630000000000004</v>
       </c>
       <c r="M30" s="3">
         <f>Measurements!M30/10</f>
@@ -3454,7 +3492,7 @@
         <v>13941</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="3">
         <f>Measurements!B31/100</f>
         <v>308.52</v>
@@ -3469,7 +3507,7 @@
       </c>
       <c r="E31" s="3">
         <f>Measurements!E31/1000000</f>
-        <v>0.005245</v>
+        <v>5.2449999999999997E-3</v>
       </c>
       <c r="F31" s="3">
         <f>Measurements!F31</f>
@@ -3481,7 +3519,7 @@
       </c>
       <c r="H31" s="3">
         <f>Measurements!H31/1000</f>
-        <v>8.956</v>
+        <v>8.9559999999999995</v>
       </c>
       <c r="I31" s="3">
         <f>Measurements!I31</f>
@@ -3493,25 +3531,25 @@
       </c>
       <c r="K31" s="3">
         <f>Measurements!K31/100</f>
-        <v>484.63</v>
+        <v>156.38999999999999</v>
       </c>
       <c r="L31" s="3">
-        <f>Measurements!L31/100</f>
-        <v>240.38</v>
+        <f>Measurements!L31/1000</f>
+        <v>6.577</v>
       </c>
       <c r="M31" s="3">
         <f>Measurements!M31/10</f>
-        <v>8770.8</v>
+        <v>8770.7999999999993</v>
       </c>
       <c r="N31" s="3">
         <f>Measurements!N31/10</f>
         <v>14063.8</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="3">
         <f>Measurements!B32/100</f>
-        <v>268.91</v>
+        <v>268.91000000000003</v>
       </c>
       <c r="C32" s="3">
         <f>Measurements!C32/100</f>
@@ -3523,7 +3561,7 @@
       </c>
       <c r="E32" s="3">
         <f>Measurements!E32/1000000</f>
-        <v>0.005278</v>
+        <v>5.2779999999999997E-3</v>
       </c>
       <c r="F32" s="3">
         <f>Measurements!F32</f>
@@ -3531,7 +3569,7 @@
       </c>
       <c r="G32" s="3">
         <f>Measurements!G32/10</f>
-        <v>1256.6</v>
+        <v>1256.5999999999999</v>
       </c>
       <c r="H32" s="3">
         <f>Measurements!H32/1000</f>
@@ -3547,11 +3585,11 @@
       </c>
       <c r="K32" s="3">
         <f>Measurements!K32/100</f>
-        <v>486.5</v>
+        <v>155.68</v>
       </c>
       <c r="L32" s="3">
-        <f>Measurements!L32/100</f>
-        <v>250.18</v>
+        <f>Measurements!L32/1000</f>
+        <v>7.0609999999999999</v>
       </c>
       <c r="M32" s="3">
         <f>Measurements!M32/10</f>
@@ -3562,64 +3600,64 @@
         <v>10491.6</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" ref="B34:N34" si="1">AVERAGE(B3:B32)</f>
-        <v>286.3743333</v>
+        <f t="shared" ref="B34:N34" si="0">AVERAGE(B3:B32)</f>
+        <v>286.37433333333337</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="1"/>
-        <v>40.327</v>
+        <f t="shared" si="0"/>
+        <v>40.326999999999991</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="1"/>
-        <v>130250.4667</v>
+        <f t="shared" si="0"/>
+        <v>130250.46666666666</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="1"/>
-        <v>0.004956666667</v>
+        <f t="shared" si="0"/>
+        <v>4.9566666666666665E-3</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>122011.9</v>
       </c>
       <c r="G34" s="3">
-        <f t="shared" si="1"/>
-        <v>1288.613333</v>
+        <f t="shared" si="0"/>
+        <v>1288.6133333333332</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="1"/>
-        <v>7.9186</v>
+        <f t="shared" si="0"/>
+        <v>7.9185999999999979</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>330439.2</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" si="1"/>
-        <v>78588.4</v>
+        <f t="shared" si="0"/>
+        <v>78588.399999999994</v>
       </c>
       <c r="K34" s="3">
-        <f t="shared" si="1"/>
-        <v>328.3616667</v>
+        <f t="shared" si="0"/>
+        <v>159.77200000000002</v>
       </c>
       <c r="L34" s="3">
-        <f t="shared" si="1"/>
-        <v>326.3863333</v>
+        <f t="shared" si="0"/>
+        <v>6.526866666666665</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" si="1"/>
-        <v>10691.00667</v>
+        <f t="shared" si="0"/>
+        <v>10691.006666666666</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="1"/>
-        <v>10855.62</v>
-      </c>
-    </row>
-    <row r="37">
+        <f t="shared" si="0"/>
+        <v>10855.619999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>13</v>
       </c>
@@ -3627,93 +3665,93 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B38" s="3">
-        <f t="shared" ref="B38:C38" si="2">B34</f>
-        <v>286.3743333</v>
+        <f t="shared" ref="B38:C38" si="1">B34</f>
+        <v>286.37433333333337</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="2"/>
-        <v>40.327</v>
-      </c>
-    </row>
-    <row r="39">
+        <f t="shared" si="1"/>
+        <v>40.326999999999991</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="3">
         <f>D34</f>
-        <v>130250.4667</v>
+        <v>130250.46666666666</v>
       </c>
       <c r="C39" s="3">
         <f>F34</f>
         <v>122011.9</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="3">
-        <f t="shared" ref="B40:C40" si="3">G34</f>
-        <v>1288.613333</v>
+        <f t="shared" ref="B40:C40" si="2">G34</f>
+        <v>1288.6133333333332</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="3"/>
-        <v>7.9186</v>
-      </c>
-    </row>
-    <row r="41">
+        <f t="shared" si="2"/>
+        <v>7.9185999999999979</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="3">
-        <f t="shared" ref="B41:C41" si="4">I34</f>
+        <f t="shared" ref="B41:C41" si="3">I34</f>
         <v>330439.2</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="4"/>
-        <v>78588.4</v>
-      </c>
-    </row>
-    <row r="42">
+        <f t="shared" si="3"/>
+        <v>78588.399999999994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="3">
-        <f t="shared" ref="B42:C42" si="5">K34</f>
-        <v>328.3616667</v>
+        <f t="shared" ref="B42:C42" si="4">K34</f>
+        <v>159.77200000000002</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="5"/>
-        <v>326.3863333</v>
-      </c>
-    </row>
-    <row r="43">
+        <f t="shared" si="4"/>
+        <v>6.526866666666665</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="3">
-        <f t="shared" ref="B43:C43" si="6">M34</f>
-        <v>10691.00667</v>
+        <f t="shared" ref="B43:C43" si="5">M34</f>
+        <v>10691.006666666666</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="6"/>
-        <v>10855.62</v>
+        <f t="shared" si="5"/>
+        <v>10855.619999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>